<commit_message>
fixed typos in requirements and WG
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -1655,9 +1650,6 @@
     <t>moved to roles. We only keep the most important ones in this ontology</t>
   </si>
   <si>
-    <t>What is the currento job title for a person?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Person, currentJobTitle, string [examples: student, postdoc, faculty, staff]. </t>
   </si>
   <si>
@@ -1941,18 +1933,22 @@
   </si>
   <si>
     <t>Conflict, dcterms:description, [string], forPublication, Publication</t>
+  </si>
+  <si>
+    <t>What is the current job title for a person?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2133,7 +2129,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2223,6 +2219,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2251,7 +2251,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="93">
     <cellStyle name="Bad" xfId="60" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2296,6 +2296,8 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="59" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2338,6 +2340,8 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="61" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -2683,14 +2687,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.796875" customWidth="1"/>
+    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2698,13 +2702,13 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="22.75">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="18.5" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>265</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A5" s="5" t="s">
         <v>266</v>
       </c>
@@ -2729,7 +2733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>267</v>
       </c>
@@ -2740,7 +2744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>268</v>
       </c>
@@ -2751,7 +2755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>269</v>
       </c>
@@ -2762,7 +2766,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>270</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>271</v>
       </c>
@@ -2784,7 +2788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>272</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>273</v>
       </c>
@@ -2806,7 +2810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>274</v>
       </c>
@@ -2817,7 +2821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>275</v>
       </c>
@@ -2828,7 +2832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A15" s="9" t="s">
         <v>276</v>
       </c>
@@ -2842,7 +2846,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A16" s="9" t="s">
         <v>277</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A17" s="9" t="s">
         <v>278</v>
       </c>
@@ -2864,7 +2868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A18" s="5" t="s">
         <v>279</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A19" s="5" t="s">
         <v>280</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A20" s="5" t="s">
         <v>281</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.5">
       <c r="A21" s="10" t="s">
         <v>282</v>
       </c>
@@ -2911,7 +2915,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A22" s="5" t="s">
         <v>283</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A23" s="5" t="s">
         <v>284</v>
       </c>
@@ -2933,7 +2937,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A24" s="5" t="s">
         <v>285</v>
       </c>
@@ -2944,7 +2948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A25" s="5" t="s">
         <v>286</v>
       </c>
@@ -2955,7 +2959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A26" s="5" t="s">
         <v>287</v>
       </c>
@@ -2966,7 +2970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A27" s="5" t="s">
         <v>288</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.5">
       <c r="A28" s="11" t="s">
         <v>289</v>
       </c>
@@ -2991,7 +2995,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A29" s="5" t="s">
         <v>290</v>
       </c>
@@ -3002,7 +3006,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A30" s="5" t="s">
         <v>291</v>
       </c>
@@ -3013,7 +3017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.5">
       <c r="A31" s="11" t="s">
         <v>292</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A32" s="5" t="s">
         <v>293</v>
       </c>
@@ -3038,7 +3042,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A33" s="5" t="s">
         <v>294</v>
       </c>
@@ -3049,7 +3053,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A34" s="5" t="s">
         <v>295</v>
       </c>
@@ -3060,7 +3064,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A35" s="5" t="s">
         <v>296</v>
       </c>
@@ -3071,7 +3075,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A36" s="5" t="s">
         <v>297</v>
       </c>
@@ -3082,7 +3086,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.5">
       <c r="A37" s="11" t="s">
         <v>298</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.5">
       <c r="A38" s="11" t="s">
         <v>299</v>
       </c>
@@ -3110,7 +3114,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A39" s="5" t="s">
         <v>300</v>
       </c>
@@ -3124,7 +3128,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A40" s="5" t="s">
         <v>301</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A41" s="9" t="s">
         <v>302</v>
       </c>
@@ -3152,7 +3156,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A42" s="9" t="s">
         <v>303</v>
       </c>
@@ -3166,7 +3170,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.5">
       <c r="A43" s="9" t="s">
         <v>304</v>
       </c>
@@ -3180,7 +3184,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A44" s="5" t="s">
         <v>305</v>
       </c>
@@ -3194,7 +3198,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A45" s="5" t="s">
         <v>306</v>
       </c>
@@ -3206,7 +3210,7 @@
       </c>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A46" s="5" t="s">
         <v>307</v>
       </c>
@@ -3218,7 +3222,7 @@
       </c>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A47" s="5" t="s">
         <v>308</v>
       </c>
@@ -3229,7 +3233,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A48" s="5" t="s">
         <v>309</v>
       </c>
@@ -3240,7 +3244,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A49" s="5" t="s">
         <v>310</v>
       </c>
@@ -3251,7 +3255,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A50" s="5" t="s">
         <v>311</v>
       </c>
@@ -3262,7 +3266,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A51" s="5" t="s">
         <v>312</v>
       </c>
@@ -3273,7 +3277,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A52" s="5" t="s">
         <v>313</v>
       </c>
@@ -3284,7 +3288,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A53" s="5" t="s">
         <v>314</v>
       </c>
@@ -3295,7 +3299,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A54" s="5" t="s">
         <v>315</v>
       </c>
@@ -3306,7 +3310,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A55" s="5" t="s">
         <v>316</v>
       </c>
@@ -3317,7 +3321,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A56" s="5" t="s">
         <v>317</v>
       </c>
@@ -3328,7 +3332,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A57" s="5" t="s">
         <v>318</v>
       </c>
@@ -3339,7 +3343,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A58" s="5" t="s">
         <v>319</v>
       </c>
@@ -3350,7 +3354,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A59" s="5" t="s">
         <v>320</v>
       </c>
@@ -3361,7 +3365,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A60" s="5" t="s">
         <v>321</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A61" s="5" t="s">
         <v>322</v>
       </c>
@@ -3383,7 +3387,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A62" s="5" t="s">
         <v>323</v>
       </c>
@@ -3394,7 +3398,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A63" s="5" t="s">
         <v>324</v>
       </c>
@@ -3405,7 +3409,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A64" s="5" t="s">
         <v>325</v>
       </c>
@@ -3416,7 +3420,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A65" s="5" t="s">
         <v>326</v>
       </c>
@@ -3427,7 +3431,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A66" s="5" t="s">
         <v>327</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A67" s="5" t="s">
         <v>328</v>
       </c>
@@ -3449,7 +3453,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A68" s="5" t="s">
         <v>329</v>
       </c>
@@ -3460,7 +3464,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A69" s="5" t="s">
         <v>330</v>
       </c>
@@ -3471,7 +3475,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A70" s="5" t="s">
         <v>331</v>
       </c>
@@ -3482,7 +3486,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A71" s="5" t="s">
         <v>332</v>
       </c>
@@ -3493,7 +3497,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A72" s="5" t="s">
         <v>332</v>
       </c>
@@ -3504,7 +3508,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A73" s="5" t="s">
         <v>333</v>
       </c>
@@ -3515,7 +3519,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A74" s="5" t="s">
         <v>334</v>
       </c>
@@ -3526,7 +3530,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A75" s="5" t="s">
         <v>335</v>
       </c>
@@ -3537,7 +3541,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A76" s="5" t="s">
         <v>336</v>
       </c>
@@ -3548,7 +3552,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A77" s="5" t="s">
         <v>337</v>
       </c>
@@ -3559,7 +3563,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A78" s="5" t="s">
         <v>338</v>
       </c>
@@ -3570,7 +3574,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A79" s="5" t="s">
         <v>339</v>
       </c>
@@ -3581,7 +3585,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A80" s="5" t="s">
         <v>340</v>
       </c>
@@ -3592,7 +3596,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A81" s="5" t="s">
         <v>341</v>
       </c>
@@ -3603,7 +3607,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="A82" s="5" t="s">
         <v>342</v>
       </c>
@@ -3614,7 +3618,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.5">
       <c r="B83" s="5" t="s">
         <v>456</v>
       </c>
@@ -3622,7 +3626,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" ht="17.5">
       <c r="B84" s="5" t="s">
         <v>524</v>
       </c>
@@ -3630,7 +3634,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="17.5">
       <c r="B85" s="5" t="s">
         <v>525</v>
       </c>
@@ -3653,17 +3657,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>116</v>
       </c>
@@ -3671,7 +3675,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -3685,7 +3689,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>354</v>
       </c>
@@ -3696,7 +3700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>355</v>
       </c>
@@ -3704,13 +3708,13 @@
         <v>117</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>356</v>
       </c>
@@ -3718,10 +3722,10 @@
         <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>446</v>
       </c>
@@ -3732,10 +3736,10 @@
         <v>120</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>357</v>
       </c>
@@ -3746,10 +3750,10 @@
         <v>122</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>358</v>
       </c>
@@ -3760,10 +3764,10 @@
         <v>124</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>359</v>
       </c>
@@ -3774,10 +3778,10 @@
         <v>126</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>360</v>
       </c>
@@ -3788,10 +3792,10 @@
         <v>128</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>361</v>
       </c>
@@ -3802,10 +3806,10 @@
         <v>130</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>362</v>
       </c>
@@ -3816,10 +3820,10 @@
         <v>132</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>363</v>
       </c>
@@ -3830,7 +3834,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A15" s="5" t="s">
         <v>364</v>
       </c>
@@ -3841,7 +3845,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A16" s="5" t="s">
         <v>365</v>
       </c>
@@ -3852,7 +3856,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A17" s="5" t="s">
         <v>366</v>
       </c>
@@ -3863,7 +3867,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A18" s="5" t="s">
         <v>367</v>
       </c>
@@ -3874,10 +3878,10 @@
         <v>142</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A19" s="5" t="s">
         <v>368</v>
       </c>
@@ -3888,7 +3892,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A20" s="5" t="s">
         <v>369</v>
       </c>
@@ -3899,7 +3903,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A21" s="5" t="s">
         <v>370</v>
       </c>
@@ -3910,7 +3914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A22" s="5" t="s">
         <v>371</v>
       </c>
@@ -3924,7 +3928,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A23" s="5" t="s">
         <v>372</v>
       </c>
@@ -3935,7 +3939,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A24" s="5" t="s">
         <v>373</v>
       </c>
@@ -3943,13 +3947,13 @@
         <v>152</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A25" s="5" t="s">
         <v>374</v>
       </c>
@@ -3960,7 +3964,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A26" s="5" t="s">
         <v>375</v>
       </c>
@@ -3968,13 +3972,13 @@
         <v>154</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>619</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A27" s="5" t="s">
         <v>376</v>
       </c>
@@ -3985,7 +3989,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A28" s="5" t="s">
         <v>377</v>
       </c>
@@ -3996,7 +4000,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A29" s="5" t="s">
         <v>502</v>
       </c>
@@ -4007,126 +4011,126 @@
         <v>530</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="17.5">
       <c r="A30" s="16" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>509</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.5">
       <c r="A31" s="16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>510</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A32" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>517</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17.5">
       <c r="A33" s="16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>518</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17.5">
       <c r="A34" s="16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>519</v>
       </c>
       <c r="C34" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="D34" t="s">
         <v>621</v>
       </c>
-      <c r="D34" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:4" ht="17.5">
       <c r="A35" s="16" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>520</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D35" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="17.5">
       <c r="A36" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>521</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17.5">
       <c r="A37" s="16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>522</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17.5">
       <c r="A38" s="16" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>523</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.5">
+      <c r="A39" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>611</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>626</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
-        <v>591</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>612</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>627</v>
       </c>
     </row>
   </sheetData>
@@ -4144,17 +4148,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>199</v>
       </c>
@@ -4162,7 +4166,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -4176,7 +4180,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>379</v>
       </c>
@@ -4187,10 +4191,10 @@
         <v>201</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>380</v>
       </c>
@@ -4204,7 +4208,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>381</v>
       </c>
@@ -4215,7 +4219,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>382</v>
       </c>
@@ -4226,7 +4230,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>383</v>
       </c>
@@ -4240,7 +4244,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>384</v>
       </c>
@@ -4251,7 +4255,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>385</v>
       </c>
@@ -4262,7 +4266,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>386</v>
       </c>
@@ -4273,7 +4277,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>387</v>
       </c>
@@ -4284,7 +4288,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>439</v>
       </c>
@@ -4295,7 +4299,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>442</v>
       </c>
@@ -4321,24 +4325,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.296875" customWidth="1"/>
-    <col min="3" max="3" width="77.296875" customWidth="1"/>
-    <col min="4" max="4" width="26.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>265</v>
       </c>
@@ -4352,7 +4356,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>350</v>
       </c>
@@ -4360,13 +4364,13 @@
         <v>212</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>351</v>
       </c>
@@ -4380,7 +4384,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>352</v>
       </c>
@@ -4394,7 +4398,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>353</v>
       </c>
@@ -4408,7 +4412,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>388</v>
       </c>
@@ -4422,7 +4426,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>389</v>
       </c>
@@ -4436,7 +4440,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>390</v>
       </c>
@@ -4450,7 +4454,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>391</v>
       </c>
@@ -4464,7 +4468,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>392</v>
       </c>
@@ -4475,7 +4479,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>393</v>
       </c>
@@ -4486,7 +4490,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>394</v>
       </c>
@@ -4494,11 +4498,11 @@
         <v>229</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A15" s="5" t="s">
         <v>395</v>
       </c>
@@ -4506,10 +4510,10 @@
         <v>231</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A16" s="5" t="s">
         <v>396</v>
       </c>
@@ -4520,18 +4524,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A17" s="5" t="s">
         <v>397</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A18" s="5" t="s">
         <v>398</v>
       </c>
@@ -4542,7 +4546,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A19" s="5" t="s">
         <v>399</v>
       </c>
@@ -4550,10 +4554,10 @@
         <v>233</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A20" s="5" t="s">
         <v>400</v>
       </c>
@@ -4561,10 +4565,10 @@
         <v>234</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>401</v>
       </c>
@@ -4578,7 +4582,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A22" s="5" t="s">
         <v>402</v>
       </c>
@@ -4589,10 +4593,10 @@
         <v>490</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A23" s="5" t="s">
         <v>403</v>
       </c>
@@ -4603,7 +4607,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A24" s="5" t="s">
         <v>404</v>
       </c>
@@ -4614,7 +4618,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A25" s="5" t="s">
         <v>405</v>
       </c>
@@ -4625,7 +4629,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A26" s="5" t="s">
         <v>406</v>
       </c>
@@ -4633,10 +4637,10 @@
         <v>241</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A27" s="5" t="s">
         <v>407</v>
       </c>
@@ -4647,7 +4651,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>408</v>
       </c>
@@ -4658,10 +4662,10 @@
         <v>244</v>
       </c>
       <c r="D28" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A29" s="5" t="s">
         <v>409</v>
       </c>
@@ -4673,7 +4677,7 @@
       </c>
       <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A30" s="5" t="s">
         <v>410</v>
       </c>
@@ -4684,7 +4688,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A31" s="5" t="s">
         <v>411</v>
       </c>
@@ -4692,10 +4696,10 @@
         <v>248</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A32" s="5" t="s">
         <v>412</v>
       </c>
@@ -4706,21 +4710,21 @@
         <v>492</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A33" s="5" t="s">
         <v>413</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A34" s="5" t="s">
         <v>414</v>
       </c>
@@ -4731,7 +4735,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A35" s="5" t="s">
         <v>415</v>
       </c>
@@ -4739,10 +4743,10 @@
         <v>483</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A36" s="5" t="s">
         <v>416</v>
       </c>
@@ -4750,82 +4754,82 @@
         <v>481</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A37" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>482</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A38" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>434</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A39" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>433</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A40" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>435</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A41" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>436</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A42" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>437</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A43" s="5" t="s">
         <v>473</v>
       </c>
@@ -4833,10 +4837,10 @@
         <v>438</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A44" s="5" t="s">
         <v>474</v>
       </c>
@@ -4844,21 +4848,21 @@
         <v>441</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A45" s="5" t="s">
         <v>475</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A46" s="5" t="s">
         <v>476</v>
       </c>
@@ -4869,7 +4873,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A47" s="5" t="s">
         <v>484</v>
       </c>
@@ -4880,7 +4884,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A48" s="5" t="s">
         <v>489</v>
       </c>
@@ -4888,10 +4892,10 @@
         <v>491</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A49" s="5" t="s">
         <v>499</v>
       </c>
@@ -4899,49 +4903,49 @@
         <v>513</v>
       </c>
       <c r="C49" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:4" ht="17.5">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="17.5">
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="17.5">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="17.5">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="17.5">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="17.5">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="17.5">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="17.5">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="17.5">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="17.5">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="17.5">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4955,22 +4959,22 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -4984,7 +4988,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>417</v>
       </c>
@@ -4995,7 +4999,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>418</v>
       </c>
@@ -5006,7 +5010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>419</v>
       </c>
@@ -5017,7 +5021,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>420</v>
       </c>
@@ -5028,7 +5032,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>421</v>
       </c>
@@ -5042,7 +5046,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>422</v>
       </c>
@@ -5050,10 +5054,10 @@
         <v>261</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>423</v>
       </c>
@@ -5064,7 +5068,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>424</v>
       </c>
@@ -5072,10 +5076,10 @@
         <v>264</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A12" s="5" t="s">
         <v>425</v>
       </c>
@@ -5083,10 +5087,10 @@
         <v>511</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A13" s="5" t="s">
         <v>494</v>
       </c>
@@ -5094,10 +5098,10 @@
         <v>512</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
       <c r="A14" s="5" t="s">
         <v>495</v>
       </c>
@@ -5105,10 +5109,10 @@
         <v>497</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.5">
       <c r="A15" s="11" t="s">
         <v>496</v>
       </c>
@@ -5116,7 +5120,7 @@
         <v>500</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -5133,23 +5137,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="59.09765625" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>445</v>
       </c>
@@ -5157,7 +5161,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -5171,7 +5175,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="16" t="s">
         <v>503</v>
       </c>
@@ -5179,130 +5183,136 @@
         <v>504</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="17.5">
       <c r="A5" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>505</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="17.5">
       <c r="A6" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>506</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="17.5">
       <c r="A7" s="16" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>507</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" s="16" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" s="16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>215</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" s="16" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" s="16" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>218</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="17.5">
       <c r="A12" s="16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.5">
       <c r="A13" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.5">
       <c r="A14" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.35">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="17.5">
       <c r="B18" s="5" t="s">
         <v>508</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5314,19 +5324,19 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="22.75">
       <c r="B1" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>445</v>
       </c>
@@ -5334,7 +5344,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="18.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -5348,7 +5358,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>354</v>
       </c>
@@ -5360,7 +5370,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>355</v>
       </c>
@@ -5372,7 +5382,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="17.5">
       <c r="A6" s="5" t="s">
         <v>356</v>
       </c>
@@ -5384,7 +5394,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="17.5">
       <c r="A7" s="5" t="s">
         <v>446</v>
       </c>
@@ -5396,7 +5406,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="17.5">
       <c r="A8" s="5" t="s">
         <v>357</v>
       </c>
@@ -5408,7 +5418,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="17.5">
       <c r="A9" s="5" t="s">
         <v>358</v>
       </c>
@@ -5420,7 +5430,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="17.5">
       <c r="A10" s="5" t="s">
         <v>359</v>
       </c>
@@ -5432,7 +5442,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="17.5">
       <c r="A11" s="5" t="s">
         <v>360</v>
       </c>
@@ -5444,7 +5454,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="17.5">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>

</xml_diff>

<commit_message>
added more protocol requirments
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="634">
   <si>
     <t>Requirement</t>
   </si>
@@ -1387,9 +1387,6 @@
   </si>
   <si>
     <t>What is the protocol description?</t>
-  </si>
-  <si>
-    <t>What are the outputs of a protocol?</t>
   </si>
   <si>
     <t>What are the data types used in a protocol?</t>
@@ -1937,6 +1934,21 @@
   <si>
     <t>What is the current job title for a person?</t>
   </si>
+  <si>
+    <t>What is the physical link to the protocol?</t>
+  </si>
+  <si>
+    <t>who ran a protocol for cohort A</t>
+  </si>
+  <si>
+    <t>What is the version of the protocol?</t>
+  </si>
+  <si>
+    <t>What is the protocol category (image genetic)?</t>
+  </si>
+  <si>
+    <t>What are the output features of a protocol?</t>
+  </si>
 </sst>
 </file>
 
@@ -1948,7 +1960,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2694,7 +2705,7 @@
     <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2702,13 +2713,13 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.75">
+    <row r="2" spans="1:4" ht="22">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.5" thickBot="1">
+    <row r="4" spans="1:4" ht="19" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>265</v>
       </c>
@@ -2722,7 +2733,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A5" s="5" t="s">
         <v>266</v>
       </c>
@@ -2733,7 +2744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
         <v>267</v>
       </c>
@@ -2744,7 +2755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
         <v>268</v>
       </c>
@@ -2755,7 +2766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
         <v>269</v>
       </c>
@@ -2766,7 +2777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>270</v>
       </c>
@@ -2777,7 +2788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
         <v>271</v>
       </c>
@@ -2788,7 +2799,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
         <v>272</v>
       </c>
@@ -2799,7 +2810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>273</v>
       </c>
@@ -2810,7 +2821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
         <v>274</v>
       </c>
@@ -2821,7 +2832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
         <v>275</v>
       </c>
@@ -2832,7 +2843,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A15" s="9" t="s">
         <v>276</v>
       </c>
@@ -2846,7 +2857,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A16" s="9" t="s">
         <v>277</v>
       </c>
@@ -2857,7 +2868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A17" s="9" t="s">
         <v>278</v>
       </c>
@@ -2868,7 +2879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
         <v>279</v>
       </c>
@@ -2879,7 +2890,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
         <v>280</v>
       </c>
@@ -2890,7 +2901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
         <v>281</v>
       </c>
@@ -2901,7 +2912,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.5">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="16">
       <c r="A21" s="10" t="s">
         <v>282</v>
       </c>
@@ -2909,13 +2920,13 @@
         <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
         <v>283</v>
       </c>
@@ -2926,7 +2937,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
         <v>284</v>
       </c>
@@ -2937,7 +2948,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
         <v>285</v>
       </c>
@@ -2948,7 +2959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
         <v>286</v>
       </c>
@@ -2959,7 +2970,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
         <v>287</v>
       </c>
@@ -2970,7 +2981,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
         <v>288</v>
       </c>
@@ -2981,7 +2992,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.5">
+    <row r="28" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A28" s="11" t="s">
         <v>289</v>
       </c>
@@ -2995,7 +3006,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
         <v>290</v>
       </c>
@@ -3006,7 +3017,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A30" s="5" t="s">
         <v>291</v>
       </c>
@@ -3017,7 +3028,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.5">
+    <row r="31" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A31" s="11" t="s">
         <v>292</v>
       </c>
@@ -3031,7 +3042,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
         <v>293</v>
       </c>
@@ -3042,7 +3053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
         <v>294</v>
       </c>
@@ -3053,7 +3064,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A34" s="5" t="s">
         <v>295</v>
       </c>
@@ -3064,7 +3075,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
         <v>296</v>
       </c>
@@ -3075,7 +3086,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
         <v>297</v>
       </c>
@@ -3086,7 +3097,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.5">
+    <row r="37" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A37" s="11" t="s">
         <v>298</v>
       </c>
@@ -3100,7 +3111,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.5">
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A38" s="11" t="s">
         <v>299</v>
       </c>
@@ -3114,7 +3125,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
         <v>300</v>
       </c>
@@ -3128,7 +3139,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
         <v>301</v>
       </c>
@@ -3142,7 +3153,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A41" s="9" t="s">
         <v>302</v>
       </c>
@@ -3156,7 +3167,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="42" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A42" s="9" t="s">
         <v>303</v>
       </c>
@@ -3170,7 +3181,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.5">
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A43" s="9" t="s">
         <v>304</v>
       </c>
@@ -3184,7 +3195,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
         <v>305</v>
       </c>
@@ -3198,7 +3209,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A45" s="5" t="s">
         <v>306</v>
       </c>
@@ -3210,7 +3221,7 @@
       </c>
       <c r="D45" s="7"/>
     </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A46" s="5" t="s">
         <v>307</v>
       </c>
@@ -3222,7 +3233,7 @@
       </c>
       <c r="D46" s="7"/>
     </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A47" s="5" t="s">
         <v>308</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A48" s="5" t="s">
         <v>309</v>
       </c>
@@ -3244,7 +3255,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="49" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
         <v>310</v>
       </c>
@@ -3255,7 +3266,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="50" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A50" s="5" t="s">
         <v>311</v>
       </c>
@@ -3266,7 +3277,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="51" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A51" s="5" t="s">
         <v>312</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="52" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A52" s="5" t="s">
         <v>313</v>
       </c>
@@ -3288,7 +3299,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="53" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A53" s="5" t="s">
         <v>314</v>
       </c>
@@ -3299,7 +3310,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A54" s="5" t="s">
         <v>315</v>
       </c>
@@ -3310,7 +3321,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A55" s="5" t="s">
         <v>316</v>
       </c>
@@ -3321,7 +3332,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A56" s="5" t="s">
         <v>317</v>
       </c>
@@ -3332,7 +3343,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A57" s="5" t="s">
         <v>318</v>
       </c>
@@ -3343,7 +3354,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="58" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A58" s="5" t="s">
         <v>319</v>
       </c>
@@ -3354,7 +3365,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="59" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A59" s="5" t="s">
         <v>320</v>
       </c>
@@ -3365,7 +3376,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A60" s="5" t="s">
         <v>321</v>
       </c>
@@ -3376,7 +3387,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A61" s="5" t="s">
         <v>322</v>
       </c>
@@ -3387,7 +3398,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="62" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A62" s="5" t="s">
         <v>323</v>
       </c>
@@ -3398,7 +3409,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A63" s="5" t="s">
         <v>324</v>
       </c>
@@ -3409,7 +3420,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A64" s="5" t="s">
         <v>325</v>
       </c>
@@ -3420,7 +3431,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A65" s="5" t="s">
         <v>326</v>
       </c>
@@ -3431,7 +3442,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="66" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A66" s="5" t="s">
         <v>327</v>
       </c>
@@ -3442,7 +3453,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="67" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A67" s="5" t="s">
         <v>328</v>
       </c>
@@ -3453,7 +3464,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A68" s="5" t="s">
         <v>329</v>
       </c>
@@ -3464,7 +3475,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="69" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A69" s="5" t="s">
         <v>330</v>
       </c>
@@ -3475,7 +3486,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="70" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A70" s="5" t="s">
         <v>331</v>
       </c>
@@ -3486,7 +3497,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="71" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A71" s="5" t="s">
         <v>332</v>
       </c>
@@ -3497,7 +3508,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="72" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A72" s="5" t="s">
         <v>332</v>
       </c>
@@ -3508,7 +3519,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A73" s="5" t="s">
         <v>333</v>
       </c>
@@ -3519,7 +3530,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A74" s="5" t="s">
         <v>334</v>
       </c>
@@ -3530,7 +3541,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A75" s="5" t="s">
         <v>335</v>
       </c>
@@ -3541,7 +3552,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A76" s="5" t="s">
         <v>336</v>
       </c>
@@ -3552,7 +3563,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A77" s="5" t="s">
         <v>337</v>
       </c>
@@ -3563,7 +3574,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A78" s="5" t="s">
         <v>338</v>
       </c>
@@ -3574,7 +3585,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="79" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A79" s="5" t="s">
         <v>339</v>
       </c>
@@ -3585,7 +3596,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="80" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A80" s="5" t="s">
         <v>340</v>
       </c>
@@ -3596,7 +3607,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A81" s="5" t="s">
         <v>341</v>
       </c>
@@ -3607,7 +3618,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A82" s="5" t="s">
         <v>342</v>
       </c>
@@ -3618,28 +3629,28 @@
         <v>198</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.5">
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="B83" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="17.5">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16">
       <c r="B84" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16">
+      <c r="B85" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="C84" s="12" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="17.5">
-      <c r="B85" s="5" t="s">
+      <c r="C85" s="12" t="s">
         <v>525</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -3657,7 +3668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -3667,15 +3678,15 @@
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -3689,7 +3700,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>354</v>
       </c>
@@ -3700,7 +3711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
         <v>355</v>
       </c>
@@ -3708,13 +3719,13 @@
         <v>117</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
         <v>356</v>
       </c>
@@ -3722,10 +3733,10 @@
         <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
         <v>446</v>
       </c>
@@ -3736,10 +3747,10 @@
         <v>120</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
         <v>357</v>
       </c>
@@ -3750,10 +3761,10 @@
         <v>122</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>358</v>
       </c>
@@ -3764,10 +3775,10 @@
         <v>124</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
         <v>359</v>
       </c>
@@ -3778,10 +3789,10 @@
         <v>126</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
         <v>360</v>
       </c>
@@ -3792,10 +3803,10 @@
         <v>128</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>361</v>
       </c>
@@ -3806,10 +3817,10 @@
         <v>130</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
         <v>362</v>
       </c>
@@ -3820,10 +3831,10 @@
         <v>132</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
         <v>363</v>
       </c>
@@ -3834,7 +3845,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A15" s="5" t="s">
         <v>364</v>
       </c>
@@ -3845,7 +3856,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A16" s="5" t="s">
         <v>365</v>
       </c>
@@ -3856,7 +3867,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A17" s="5" t="s">
         <v>366</v>
       </c>
@@ -3867,7 +3878,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
         <v>367</v>
       </c>
@@ -3878,10 +3889,10 @@
         <v>142</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
         <v>368</v>
       </c>
@@ -3892,7 +3903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
         <v>369</v>
       </c>
@@ -3903,7 +3914,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A21" s="5" t="s">
         <v>370</v>
       </c>
@@ -3914,7 +3925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
         <v>371</v>
       </c>
@@ -3925,10 +3936,10 @@
         <v>149</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
         <v>372</v>
       </c>
@@ -3939,7 +3950,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
         <v>373</v>
       </c>
@@ -3947,13 +3958,13 @@
         <v>152</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>616</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
         <v>374</v>
       </c>
@@ -3964,7 +3975,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
         <v>375</v>
       </c>
@@ -3972,13 +3983,13 @@
         <v>154</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
         <v>376</v>
       </c>
@@ -3989,7 +4000,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A28" s="5" t="s">
         <v>377</v>
       </c>
@@ -4000,137 +4011,137 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16">
+      <c r="A30" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A32" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16">
+      <c r="A34" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>518</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>619</v>
+      </c>
+      <c r="D34" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16">
+      <c r="A35" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="D35" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.5">
-      <c r="A30" s="16" t="s">
-        <v>581</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.5">
-      <c r="A31" s="16" t="s">
-        <v>582</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A32" s="5" t="s">
-        <v>583</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="C32" s="5" t="s">
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16">
+      <c r="A37" s="16" t="s">
+        <v>587</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16">
+      <c r="A38" s="16" t="s">
+        <v>588</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>623</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17.5">
-      <c r="A33" s="16" t="s">
-        <v>584</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.5">
-      <c r="A34" s="16" t="s">
-        <v>585</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="D34" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17.5">
-      <c r="A35" s="16" t="s">
-        <v>586</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="D35" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17.5">
-      <c r="A36" s="16" t="s">
-        <v>587</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17.5">
-      <c r="A37" s="16" t="s">
-        <v>588</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="C37" s="5" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="16">
+      <c r="A39" s="16" t="s">
+        <v>589</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="17.5">
-      <c r="A38" s="16" t="s">
-        <v>589</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="16" t="s">
         <v>625</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.5">
-      <c r="A39" s="16" t="s">
-        <v>590</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>611</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -4158,7 +4169,7 @@
     <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>199</v>
       </c>
@@ -4166,7 +4177,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -4180,7 +4191,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>379</v>
       </c>
@@ -4191,10 +4202,10 @@
         <v>201</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
         <v>380</v>
       </c>
@@ -4202,13 +4213,13 @@
         <v>202</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
         <v>381</v>
       </c>
@@ -4216,10 +4227,10 @@
         <v>203</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
         <v>382</v>
       </c>
@@ -4227,10 +4238,10 @@
         <v>204</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
         <v>383</v>
       </c>
@@ -4238,13 +4249,13 @@
         <v>205</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>384</v>
       </c>
@@ -4252,10 +4263,10 @@
         <v>206</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
         <v>385</v>
       </c>
@@ -4263,10 +4274,10 @@
         <v>207</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
         <v>386</v>
       </c>
@@ -4274,10 +4285,10 @@
         <v>208</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>387</v>
       </c>
@@ -4285,10 +4296,10 @@
         <v>209</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
         <v>439</v>
       </c>
@@ -4296,18 +4307,18 @@
         <v>440</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
         <v>442</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -4337,12 +4348,12 @@
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>265</v>
       </c>
@@ -4356,7 +4367,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>350</v>
       </c>
@@ -4364,13 +4375,13 @@
         <v>212</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
         <v>351</v>
       </c>
@@ -4381,10 +4392,10 @@
         <v>214</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
         <v>352</v>
       </c>
@@ -4395,10 +4406,10 @@
         <v>216</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
         <v>353</v>
       </c>
@@ -4409,10 +4420,10 @@
         <v>217</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
         <v>388</v>
       </c>
@@ -4423,10 +4434,10 @@
         <v>223</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>389</v>
       </c>
@@ -4437,10 +4448,10 @@
         <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
         <v>390</v>
       </c>
@@ -4451,10 +4462,10 @@
         <v>225</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
         <v>391</v>
       </c>
@@ -4465,10 +4476,10 @@
         <v>227</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>392</v>
       </c>
@@ -4479,7 +4490,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
         <v>393</v>
       </c>
@@ -4487,10 +4498,10 @@
         <v>228</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
         <v>394</v>
       </c>
@@ -4498,11 +4509,11 @@
         <v>229</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A15" s="5" t="s">
         <v>395</v>
       </c>
@@ -4510,10 +4521,10 @@
         <v>231</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A16" s="5" t="s">
         <v>396</v>
       </c>
@@ -4524,18 +4535,18 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A17" s="5" t="s">
         <v>397</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>578</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.5">
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
         <v>398</v>
       </c>
@@ -4546,7 +4557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
         <v>399</v>
       </c>
@@ -4554,10 +4565,10 @@
         <v>233</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
         <v>400</v>
       </c>
@@ -4565,7 +4576,7 @@
         <v>234</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4579,10 +4590,10 @@
         <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
         <v>402</v>
       </c>
@@ -4590,13 +4601,13 @@
         <v>237</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
         <v>403</v>
       </c>
@@ -4604,10 +4615,10 @@
         <v>238</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
         <v>404</v>
       </c>
@@ -4615,10 +4626,10 @@
         <v>239</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
         <v>405</v>
       </c>
@@ -4629,7 +4640,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
         <v>406</v>
       </c>
@@ -4637,10 +4648,10 @@
         <v>241</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
         <v>407</v>
       </c>
@@ -4648,7 +4659,7 @@
         <v>242</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4662,10 +4673,10 @@
         <v>244</v>
       </c>
       <c r="D28" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
         <v>409</v>
       </c>
@@ -4673,11 +4684,11 @@
         <v>245</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D29" s="14"/>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A30" s="5" t="s">
         <v>410</v>
       </c>
@@ -4688,7 +4699,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A31" s="5" t="s">
         <v>411</v>
       </c>
@@ -4696,10 +4707,10 @@
         <v>248</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
         <v>412</v>
       </c>
@@ -4707,240 +4718,240 @@
         <v>249</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
         <v>413</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A34" s="5" t="s">
         <v>414</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.5">
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
         <v>415</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
         <v>416</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A37" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C37" s="16" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A38" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A38" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>434</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>433</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>435</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A41" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>436</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A42" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>437</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A43" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>438</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>441</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A45" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>628</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A46" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>629</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B46" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A47" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A48" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A49" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C49" s="16" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A46" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A47" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A48" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A49" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="C49" s="16" t="s">
+      <c r="D49" s="5" t="s">
         <v>535</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.5">
+    </row>
+    <row r="50" spans="1:4" ht="16">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="17.5">
+    <row r="51" spans="1:4" ht="16">
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="17.5">
+    <row r="52" spans="1:4" ht="16">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="17.5">
+    <row r="53" spans="1:4" ht="16">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="17.5">
+    <row r="54" spans="1:4" ht="16">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="17.5">
+    <row r="55" spans="1:4" ht="16">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="17.5">
+    <row r="56" spans="1:4" ht="16">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="17.5">
+    <row r="57" spans="1:4" ht="16">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="17.5">
+    <row r="58" spans="1:4" ht="16">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="17.5">
+    <row r="59" spans="1:4" ht="16">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="17.5">
+    <row r="60" spans="1:4" ht="16">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
@@ -4969,12 +4980,12 @@
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -4988,7 +4999,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>417</v>
       </c>
@@ -4999,7 +5010,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
         <v>418</v>
       </c>
@@ -5010,7 +5021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
         <v>419</v>
       </c>
@@ -5018,10 +5029,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
         <v>420</v>
       </c>
@@ -5029,24 +5040,24 @@
         <v>260</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
         <v>421</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
         <v>422</v>
       </c>
@@ -5054,10 +5065,10 @@
         <v>261</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
         <v>423</v>
       </c>
@@ -5068,7 +5079,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.5">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
         <v>424</v>
       </c>
@@ -5076,51 +5087,51 @@
         <v>264</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.5">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
         <v>425</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A13" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.5">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:4" s="11" customFormat="1" ht="16">
+      <c r="A15" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.5">
-      <c r="A15" s="11" t="s">
-        <v>496</v>
-      </c>
       <c r="B15" s="11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -5137,7 +5148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -5148,7 +5159,7 @@
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>443</v>
       </c>
@@ -5161,7 +5172,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -5175,134 +5186,134 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="18" thickTop="1">
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="16" t="s">
+        <v>502</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>503</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C4" s="16" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A5" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>504</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="17.5">
-      <c r="A5" s="16" t="s">
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A6" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="16" t="s">
         <v>505</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C6" s="16" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A7" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>506</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="17.5">
-      <c r="A6" s="16" t="s">
-        <v>567</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>506</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="17.5">
-      <c r="A7" s="16" t="s">
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="16" t="s">
         <v>568</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>507</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.5">
-      <c r="A8" s="16" t="s">
-        <v>569</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="17.5">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" s="16" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>215</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" s="16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" s="16" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>218</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5">
+    <row r="12" spans="1:4" ht="16">
       <c r="A12" s="16" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.5">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
       <c r="A13" s="16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17.5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="17.5">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="16">
       <c r="B18" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -5318,10 +5329,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5331,7 +5342,7 @@
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.75">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>443</v>
       </c>
@@ -5344,7 +5355,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.5" thickBot="1">
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>265</v>
       </c>
@@ -5358,7 +5369,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1">
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>354</v>
       </c>
@@ -5368,9 +5379,11 @@
       <c r="C4" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.5">
+      <c r="D4" s="5" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
       <c r="A5" s="5" t="s">
         <v>355</v>
       </c>
@@ -5382,7 +5395,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" ht="17.5">
+    <row r="6" spans="1:4" ht="16">
       <c r="A6" s="5" t="s">
         <v>356</v>
       </c>
@@ -5394,7 +5407,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="17.5">
+    <row r="7" spans="1:4" ht="16">
       <c r="A7" s="5" t="s">
         <v>446</v>
       </c>
@@ -5406,7 +5419,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="17.5">
+    <row r="8" spans="1:4" ht="16">
       <c r="A8" s="5" t="s">
         <v>357</v>
       </c>
@@ -5418,7 +5431,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="17.5">
+    <row r="9" spans="1:4" ht="16">
       <c r="A9" s="5" t="s">
         <v>358</v>
       </c>
@@ -5430,33 +5443,62 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="17.5">
+    <row r="10" spans="1:4" ht="16">
       <c r="A10" s="5" t="s">
         <v>359</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>454</v>
+        <v>633</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>448</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="17.5">
+    <row r="11" spans="1:4" ht="16">
       <c r="A11" s="5" t="s">
         <v>360</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>448</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="17.5">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>448</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding prelim protocol ont
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="650">
   <si>
     <t>Requirement</t>
   </si>
@@ -1366,9 +1366,6 @@
   </si>
   <si>
     <t>Pr4</t>
-  </si>
-  <si>
-    <t>Who run a protocol?</t>
   </si>
   <si>
     <t>TBD</t>
@@ -1944,10 +1941,61 @@
     <t>What is the version of the protocol?</t>
   </si>
   <si>
-    <t>What is the protocol category (image genetic)?</t>
-  </si>
-  <si>
     <t>What are the output features of a protocol?</t>
+  </si>
+  <si>
+    <t>Who ran a protocol?</t>
+  </si>
+  <si>
+    <t>Project, usesProtocol, Protocol</t>
+  </si>
+  <si>
+    <t>Cohort, hasRunProtocol, Protocol</t>
+  </si>
+  <si>
+    <t>Protocol, hasContact, Person</t>
+  </si>
+  <si>
+    <t>Protocol, dcterms:title, [string literal]</t>
+  </si>
+  <si>
+    <t>Protocol, hasDescription, [string]</t>
+  </si>
+  <si>
+    <t>Protocol, hasOutputFeature, [string]</t>
+  </si>
+  <si>
+    <t>Procotol, hasDataType, [string]</t>
+  </si>
+  <si>
+    <t>Protocol, hasLink, [string]</t>
+  </si>
+  <si>
+    <t>Protocol, hasVersion, [string]</t>
+  </si>
+  <si>
+    <t>Are there more protocol categories</t>
+  </si>
+  <si>
+    <t>What is the protocol category (imaging genetic)?</t>
+  </si>
+  <si>
+    <t>Protocol, hasCategory, {Imaging, Genetic}</t>
+  </si>
+  <si>
+    <t>Protocol, hasType, [string]</t>
+  </si>
+  <si>
+    <t>Should data type be a class</t>
+  </si>
+  <si>
+    <t>Should output feature be a class</t>
+  </si>
+  <si>
+    <t>Should type be a class</t>
+  </si>
+  <si>
+    <t>What is the type of procedure that a protocol represents?</t>
   </si>
 </sst>
 </file>
@@ -2140,7 +2188,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2234,6 +2282,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2262,7 +2314,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="97">
     <cellStyle name="Bad" xfId="60" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2309,6 +2361,8 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="59" builtinId="26"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2353,6 +2407,8 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="61" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -2920,7 +2976,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>344</v>
@@ -3631,26 +3687,26 @@
     </row>
     <row r="83" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="B83" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="16">
       <c r="B84" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="16">
       <c r="B85" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="C85" s="12" t="s">
         <v>524</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>525</v>
       </c>
     </row>
   </sheetData>
@@ -3683,7 +3739,7 @@
         <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
@@ -3719,10 +3775,10 @@
         <v>117</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3733,7 +3789,7 @@
         <v>118</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3747,7 +3803,7 @@
         <v>120</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3761,7 +3817,7 @@
         <v>122</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3775,7 +3831,7 @@
         <v>124</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3789,7 +3845,7 @@
         <v>126</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3803,7 +3859,7 @@
         <v>128</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3817,7 +3873,7 @@
         <v>130</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3831,7 +3887,7 @@
         <v>132</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3889,7 +3945,7 @@
         <v>142</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3936,7 +3992,7 @@
         <v>149</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3958,10 +4014,10 @@
         <v>152</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>615</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3983,10 +4039,10 @@
         <v>154</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>617</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4013,135 +4069,135 @@
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
       <c r="A30" s="16" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16">
       <c r="A31" s="16" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" s="16" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
       <c r="A34" s="16" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C34" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="D34" t="s">
         <v>619</v>
-      </c>
-      <c r="D34" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16">
       <c r="A35" s="16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D35" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" s="16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16">
       <c r="A37" s="16" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16">
       <c r="A39" s="16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
@@ -4202,7 +4258,7 @@
         <v>201</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4213,10 +4269,10 @@
         <v>202</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4227,7 +4283,7 @@
         <v>203</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4238,7 +4294,7 @@
         <v>204</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4249,10 +4305,10 @@
         <v>205</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4263,7 +4319,7 @@
         <v>206</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4274,7 +4330,7 @@
         <v>207</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4285,7 +4341,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4296,7 +4352,7 @@
         <v>209</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4307,7 +4363,7 @@
         <v>440</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4315,10 +4371,10 @@
         <v>442</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -4337,7 +4393,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4375,10 +4431,10 @@
         <v>212</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4392,7 +4448,7 @@
         <v>214</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4406,7 +4462,7 @@
         <v>216</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4420,7 +4476,7 @@
         <v>217</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4434,7 +4490,7 @@
         <v>223</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4448,7 +4504,7 @@
         <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4462,7 +4518,7 @@
         <v>225</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4476,7 +4532,7 @@
         <v>227</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4498,7 +4554,7 @@
         <v>228</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4509,7 +4565,7 @@
         <v>229</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D14" s="16"/>
     </row>
@@ -4521,7 +4577,7 @@
         <v>231</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4540,10 +4596,10 @@
         <v>397</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="C17" s="16" t="s">
         <v>577</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4565,7 +4621,7 @@
         <v>233</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4576,7 +4632,7 @@
         <v>234</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4590,7 +4646,7 @@
         <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4601,10 +4657,10 @@
         <v>237</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4615,7 +4671,7 @@
         <v>238</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4626,7 +4682,7 @@
         <v>239</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4648,7 +4704,7 @@
         <v>241</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4659,7 +4715,7 @@
         <v>242</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4673,7 +4729,7 @@
         <v>244</v>
       </c>
       <c r="D28" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4684,7 +4740,7 @@
         <v>245</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D29" s="14"/>
     </row>
@@ -4707,7 +4763,7 @@
         <v>248</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4718,10 +4774,10 @@
         <v>249</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4729,10 +4785,10 @@
         <v>413</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4740,10 +4796,10 @@
         <v>414</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>484</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4751,10 +4807,10 @@
         <v>415</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4762,162 +4818,162 @@
         <v>416</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A37" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A38" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>434</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>433</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>435</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A41" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>436</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A42" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>437</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A43" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>438</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>441</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A45" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A46" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A47" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A48" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C49" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>534</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16">
@@ -4970,7 +5026,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5029,7 +5085,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5040,7 +5096,7 @@
         <v>260</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5048,13 +5104,13 @@
         <v>421</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5065,7 +5121,7 @@
         <v>261</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5087,7 +5143,7 @@
         <v>264</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5095,43 +5151,43 @@
         <v>425</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A15" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -5188,132 +5244,132 @@
     </row>
     <row r="4" spans="1:4" s="16" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>503</v>
-      </c>
       <c r="C4" s="16" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="16" customFormat="1" ht="16">
       <c r="A5" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="16" customFormat="1" ht="16">
       <c r="A6" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="16" customFormat="1" ht="16">
       <c r="A7" s="16" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16">
       <c r="A8" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>213</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="16">
       <c r="A9" s="16" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>215</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="16">
       <c r="A10" s="16" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>221</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" s="16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>218</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="16" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>219</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="16" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>220</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16">
       <c r="A14" s="16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>222</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="16">
       <c r="B18" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -5329,10 +5385,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5374,13 +5430,13 @@
         <v>354</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
@@ -5388,10 +5444,10 @@
         <v>355</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>448</v>
+        <v>634</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -5400,10 +5456,10 @@
         <v>356</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>448</v>
+        <v>633</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -5412,10 +5468,10 @@
         <v>446</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>448</v>
+        <v>635</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -5424,10 +5480,10 @@
         <v>357</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>448</v>
+        <v>636</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -5436,46 +5492,50 @@
         <v>358</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" s="13" customFormat="1">
+      <c r="A10" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>631</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>638</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="13" customFormat="1">
+      <c r="A11" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>633</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="D11" s="5"/>
+      <c r="C11" s="13" t="s">
+        <v>639</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>646</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="5" t="s">
         <v>361</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>448</v>
+        <v>640</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
@@ -5483,25 +5543,43 @@
         <v>362</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="5" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="13" customFormat="1">
+      <c r="A14" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>448</v>
+      <c r="B14" s="13" t="s">
+        <v>643</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>644</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="13" customFormat="1">
+      <c r="A15" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>649</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>645</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>648</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
fixed range of hasCategory for protocol
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="649">
   <si>
     <t>Requirement</t>
   </si>
@@ -1974,15 +1974,9 @@
     <t>Protocol, hasVersion, [string]</t>
   </si>
   <si>
-    <t>Are there more protocol categories</t>
-  </si>
-  <si>
     <t>What is the protocol category (imaging genetic)?</t>
   </si>
   <si>
-    <t>Protocol, hasCategory, {Imaging, Genetic}</t>
-  </si>
-  <si>
     <t>Protocol, hasType, [string]</t>
   </si>
   <si>
@@ -1996,6 +1990,9 @@
   </si>
   <si>
     <t>What is the type of procedure that a protocol represents?</t>
+  </si>
+  <si>
+    <t>Protocol, hasCategory, [string]</t>
   </si>
 </sst>
 </file>
@@ -2008,6 +2005,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5388,7 +5386,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5510,7 +5508,7 @@
         <v>638</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1">
@@ -5524,7 +5522,7 @@
         <v>639</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
@@ -5549,18 +5547,15 @@
         <v>641</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="13" customFormat="1">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>363</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>643</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>644</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="B14" t="s">
         <v>642</v>
+      </c>
+      <c r="C14" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="13" customFormat="1">
@@ -5568,13 +5563,13 @@
         <v>364</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIxed title metadata and requirements
In next commits will remove redundancies between vocabularies.
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="660">
   <si>
     <t>Requirement</t>
   </si>
@@ -225,13 +230,7 @@
     <t>Describing the projects a cohort is part of</t>
   </si>
   <si>
-    <t>Cohort, isCohortInProject, Project</t>
-  </si>
-  <si>
     <t>Describing the working groups the cohort is part of</t>
-  </si>
-  <si>
-    <t>Cohort, isCohortInWorkingGroup, WorkingGroup</t>
   </si>
   <si>
     <t>Describing the method for obtaining the patient information of a cohort</t>
@@ -1554,9 +1553,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>Who contributed to writing a paper?</t>
-  </si>
-  <si>
     <t>Who contributed to the design of a project?</t>
   </si>
   <si>
@@ -1566,9 +1562,6 @@
     <t>Who read the paper?</t>
   </si>
   <si>
-    <t>Should have as domain a project/Paper and range person</t>
-  </si>
-  <si>
     <t>Which author has a conflict in a publication?</t>
   </si>
   <si>
@@ -1695,9 +1688,6 @@
     <t>AcademicArticle, author, Person</t>
   </si>
   <si>
-    <t>we created enigma:Person, equivalent to foaf:Person, to address these requirements</t>
-  </si>
-  <si>
     <t>Person, foaf:mbox, URI (range is a resource)</t>
   </si>
   <si>
@@ -1830,39 +1820,12 @@
     <t>WorkingGroup, rdf:type, [HealthyVariation,  GeneticStudy, Methodology, ClinicalPopulation]</t>
   </si>
   <si>
-    <t>Project,hasDataAnalyst, Person</t>
-  </si>
-  <si>
-    <t>Project,hasGeneticDataAnalyst, Person</t>
-  </si>
-  <si>
-    <t>Project,hasImagingDataAnalyst, Person</t>
-  </si>
-  <si>
-    <t>Project,hasDataCollector, Person</t>
-  </si>
-  <si>
-    <t>Project,hasGeneticDataCollector, Person</t>
-  </si>
-  <si>
-    <t>Project,hasImagingDataCollector, Person</t>
-  </si>
-  <si>
     <t>Project,hasDeveloper, Person</t>
   </si>
   <si>
-    <t>AcademicArticle, dcterms:contributor, author, Person</t>
-  </si>
-  <si>
     <t>Project,hasDesigner, Person</t>
   </si>
   <si>
-    <t>AcademicArticle,hasReviewer, Person</t>
-  </si>
-  <si>
-    <t>AcademicArticle,firstDraftContributor, Person</t>
-  </si>
-  <si>
     <t>AcademicArticle, http://purl.org/dc/terms/title</t>
   </si>
   <si>
@@ -1993,13 +1956,88 @@
   </si>
   <si>
     <t>Protocol, hasCategory, [string]</t>
+  </si>
+  <si>
+    <t>Project, Cohort,hasDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Cohort,Project,hasGeneticDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Cohort,Project,hasImagingDataAnalyst, Person</t>
+  </si>
+  <si>
+    <t>Cohort,hasDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Cohort,hasGeneticDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Cohort,hasImagingDataCollector, Person</t>
+  </si>
+  <si>
+    <t>Describing the cohorts/projects a person is a data analyst of</t>
+  </si>
+  <si>
+    <t>Describing the cohorts/projects a person is a genetic data analyst of</t>
+  </si>
+  <si>
+    <t>Describing the cohorts/projects a person is an imaging data analyst of</t>
+  </si>
+  <si>
+    <t>Describing the cohorts a person is a data collector of</t>
+  </si>
+  <si>
+    <t>Describing the cohorts a person is a genetic data collector of</t>
+  </si>
+  <si>
+    <t>Describing the cohorts a person is an imaging data collector of</t>
+  </si>
+  <si>
+    <t>Project,AcademicArticle, dcterms:contributor, author, Person</t>
+  </si>
+  <si>
+    <t>Project,AcademicArticle,firstDraftContributor, Person</t>
+  </si>
+  <si>
+    <t>Project,AcademicArticle,hasReviewer, Person</t>
+  </si>
+  <si>
+    <t>Neda thinks this term is not useful because it is coveredby "investigator". It also refers to cohorts, not projects. 3-23-2018</t>
+  </si>
+  <si>
+    <t>moved to roles ontology. Collectors are from Cohorts only, not projects (Neda, 3-23-2018)</t>
+  </si>
+  <si>
+    <t>moved to Roles</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Who is the last lead of a project (i.e., the person who should be the last author)</t>
+  </si>
+  <si>
+    <t>Project, AcademicArticle, hasLastLead, Person</t>
+  </si>
+  <si>
+    <t>Agreed on 3-23-2018 to distinguish leads from the senior leads of a project. Avoided the term "senior" in purpose</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>Moved to roles. For convenience in the wiki, we extend contributor with Enigma:contributor, with domain enigma:Person. We created enigma:Person, equivalent to foaf:Person, to address these requirements</t>
+  </si>
+  <si>
+    <t>Who contributed to writing a paper, or a project?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2748,34 +2786,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22.8">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" thickBot="1">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2784,12 +2822,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A5" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -2798,9 +2836,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
@@ -2809,9 +2847,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -2820,9 +2858,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -2831,9 +2869,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
@@ -2842,9 +2880,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A10" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -2853,9 +2891,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A11" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -2864,9 +2902,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -2875,9 +2913,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
@@ -2886,9 +2924,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -2897,9 +2935,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
       <c r="A15" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>27</v>
@@ -2908,12 +2946,12 @@
         <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="16">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
       <c r="A16" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>29</v>
@@ -2922,9 +2960,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
       <c r="A17" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
@@ -2933,9 +2971,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A18" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
@@ -2944,9 +2982,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A19" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>35</v>
@@ -2955,9 +2993,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A20" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
@@ -2966,23 +3004,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="16">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.399999999999999">
       <c r="A21" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A22" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>40</v>
@@ -2991,20 +3029,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A23" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A24" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>46</v>
@@ -3013,9 +3051,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A25" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>47</v>
@@ -3024,9 +3062,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A26" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>48</v>
@@ -3035,9 +3073,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A27" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
@@ -3046,9 +3084,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="11" customFormat="1" ht="16">
+    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
       <c r="A28" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>52</v>
@@ -3057,12 +3095,12 @@
         <v>53</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A29" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -3071,9 +3109,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A30" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>56</v>
@@ -3082,9 +3120,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="11" customFormat="1" ht="16">
+    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
       <c r="A31" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>58</v>
@@ -3093,12 +3131,12 @@
         <v>3</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A32" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>59</v>
@@ -3107,9 +3145,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A33" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>61</v>
@@ -3118,9 +3156,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A34" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>63</v>
@@ -3129,582 +3167,582 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A35" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A36" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A36" s="5" t="s">
+      <c r="C36" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+      <c r="A37" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+      <c r="A38" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="11" customFormat="1" ht="16">
-      <c r="A37" s="11" t="s">
+      <c r="B38" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A39" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="11" customFormat="1" ht="16">
-      <c r="A38" s="11" t="s">
+      <c r="B39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A40" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A39" s="5" t="s">
+      <c r="B40" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+      <c r="A41" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="B41" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A40" s="5" t="s">
+    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+      <c r="A42" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B42" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="C42" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A41" s="9" t="s">
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+      <c r="A43" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B43" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D43" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A44" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A42" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="B42" s="9" t="s">
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A45" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A46" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A47" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C47" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="9" customFormat="1" ht="16">
-      <c r="A43" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="B43" s="9" t="s">
+    </row>
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A48" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C48" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A44" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A45" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A46" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A47" s="5" t="s">
+    </row>
+    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A49" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C49" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A48" s="5" t="s">
+    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A50" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A49" s="5" t="s">
+    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A51" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B51" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C51" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A52" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A53" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A54" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A55" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A56" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A57" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A58" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A59" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A60" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A61" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A62" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A63" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A64" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A65" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A66" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A67" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A50" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="5" t="s">
+    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A68" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A51" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A52" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A53" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A54" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A55" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A56" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A57" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A58" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A59" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A60" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A61" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A62" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A63" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A64" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A65" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="5" t="s">
+    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A69" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A66" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="5" t="s">
+    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A70" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A67" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="5" t="s">
+    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A71" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A68" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="5" t="s">
+    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A72" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A69" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C69" s="5" t="s">
+    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A73" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A74" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A75" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A76" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" s="5" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A70" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C70" s="5" t="s">
+    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A77" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A71" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A72" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A73" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A74" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A75" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A76" s="5" t="s">
+    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A78" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A77" s="5" t="s">
+    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A79" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A78" s="5" t="s">
+    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A80" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A79" s="5" t="s">
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A81" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A80" s="5" t="s">
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A82" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B82" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C82" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A81" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="5" customFormat="1" ht="16">
-      <c r="A82" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
       <c r="B83" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="16">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17.399999999999999">
       <c r="B84" s="5" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="16">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17.399999999999999">
       <c r="B85" s="5" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -3722,27 +3760,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3751,12 +3789,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3765,437 +3803,437 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A6" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A7" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A8" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>574</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A6" s="5" t="s">
+      <c r="B8" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A9" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A8" s="5" t="s">
+      <c r="B9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A10" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="B10" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A11" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
+      <c r="B11" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A12" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
+      <c r="B12" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A13" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A12" s="5" t="s">
+      <c r="B13" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A14" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A13" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A15" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A14" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A16" s="5" t="s">
         <v>363</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A15" s="5" t="s">
+      <c r="B16" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A17" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A18" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A17" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A19" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A18" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A20" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A19" s="5" t="s">
+      <c r="B20" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A21" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A20" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A21" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A22" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A23" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A24" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="B24" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A25" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A26" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A27" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A28" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A29" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17.399999999999999">
+      <c r="A30" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17.399999999999999">
+      <c r="A31" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A32" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17.399999999999999">
+      <c r="A33" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17.399999999999999">
+      <c r="A34" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="D34" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17.399999999999999">
+      <c r="A35" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A23" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A24" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A25" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A26" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>616</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A27" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A28" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A29" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16">
-      <c r="A30" s="16" t="s">
-        <v>579</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16">
-      <c r="A31" s="16" t="s">
+      <c r="C35" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="D35" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17.399999999999999">
+      <c r="A36" s="16" t="s">
         <v>580</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A32" s="5" t="s">
+      <c r="B36" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17.399999999999999">
+      <c r="A37" s="16" t="s">
         <v>581</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16">
-      <c r="A33" s="16" t="s">
+      <c r="B37" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17.399999999999999">
+      <c r="A38" s="16" t="s">
         <v>582</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16">
-      <c r="A34" s="16" t="s">
+      <c r="B38" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.399999999999999">
+      <c r="A39" s="16" t="s">
         <v>583</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>517</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="D34" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16">
-      <c r="A35" s="16" t="s">
-        <v>584</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>518</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>606</v>
-      </c>
-      <c r="D35" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16">
-      <c r="A36" s="16" t="s">
-        <v>585</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16">
-      <c r="A37" s="16" t="s">
-        <v>586</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>520</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16">
-      <c r="A38" s="16" t="s">
-        <v>587</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>623</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="16">
-      <c r="A39" s="16" t="s">
-        <v>588</v>
-      </c>
       <c r="B39" s="16" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -4217,23 +4255,23 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4242,137 +4280,137 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A5" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A6" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A5" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A7" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>459</v>
       </c>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A8" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A9" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A10" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A11" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A12" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A13" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A6" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A8" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="D8" s="5" t="s">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A14" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>467</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A12" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A13" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A14" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -4390,26 +4428,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.33203125" customWidth="1"/>
-    <col min="3" max="3" width="77.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.296875" customWidth="1"/>
+    <col min="3" max="3" width="77.296875" customWidth="1"/>
+    <col min="4" max="4" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4418,594 +4456,597 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+      <c r="A4" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A5" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
-      <c r="A4" s="5" t="s">
+      <c r="C5" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A6" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>546</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A7" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A6" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="B7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D7" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A8" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D8" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A9" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A8" s="5" t="s">
+      <c r="C9" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A10" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B10" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A11" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="B11" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A12" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
+      <c r="C12" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A13" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="15" t="s">
+      <c r="B13" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A14" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A12" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A13" s="5" t="s">
+      <c r="C14" s="16" t="s">
+        <v>543</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A15" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A16" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A14" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>547</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A17" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A16" s="5" t="s">
+      <c r="B17" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A18" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A17" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>576</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A18" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A19" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A20" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>399</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A22" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A23" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="C21" s="15" t="s">
+      <c r="B23" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="D21" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A22" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A24" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>488</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A23" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A25" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A26" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A27" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>475</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A24" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A25" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A26" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A27" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>406</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D28" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A29" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A30" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="C28" s="15" t="s">
+      <c r="B30" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D28" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A29" s="5" t="s">
+      <c r="C30" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A31" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B31" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A32" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A33" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A34" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A35" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A36" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A37" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A30" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A31" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A32" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>490</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A33" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A34" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="C37" s="16" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A38" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A39" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>551</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A40" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A41" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A42" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A43" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A44" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A45" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A46" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A47" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A35" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A36" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A37" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="C37" s="16" t="s">
+    </row>
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A48" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A38" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>555</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A39" s="5" t="s">
-        <v>537</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>556</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A40" s="5" t="s">
-        <v>538</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A41" s="5" t="s">
-        <v>539</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A42" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A43" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A44" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A45" s="5" t="s">
-        <v>473</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>627</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A46" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A47" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A48" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A49" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17.399999999999999">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="16">
+    <row r="51" spans="1:4" ht="17.399999999999999">
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="16">
+    <row r="52" spans="1:4" ht="17.399999999999999">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="16">
+    <row r="53" spans="1:4" ht="17.399999999999999">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="16">
+    <row r="54" spans="1:4" ht="17.399999999999999">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="16">
+    <row r="55" spans="1:4" ht="17.399999999999999">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="16">
+    <row r="56" spans="1:4" ht="17.399999999999999">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="16">
+    <row r="57" spans="1:4" ht="17.399999999999999">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="16">
+    <row r="58" spans="1:4" ht="17.399999999999999">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="16">
+    <row r="59" spans="1:4" ht="17.399999999999999">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="16">
+    <row r="60" spans="1:4" ht="17.399999999999999">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
@@ -5027,21 +5068,21 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5050,142 +5091,142 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A8" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A9" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A10" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A8" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A11" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A12" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A13" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A14" s="5" t="s">
         <v>491</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A9" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A10" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A11" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A12" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A13" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+      <c r="A15" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
-      <c r="A14" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="11" customFormat="1" ht="16">
-      <c r="A15" s="11" t="s">
-        <v>494</v>
-      </c>
       <c r="B15" s="11" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -5202,33 +5243,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="59.1640625" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.19921875" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5237,138 +5278,168 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
+      <c r="A5" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>590</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
+      <c r="A6" s="16" t="s">
+        <v>560</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>501</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="C6" s="16" t="s">
+        <v>648</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
+      <c r="A7" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="16">
-      <c r="A5" s="16" t="s">
+      <c r="C7" s="16" t="s">
+        <v>649</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.399999999999999">
+      <c r="A8" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.399999999999999">
+      <c r="A9" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.399999999999999">
+      <c r="A10" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>503</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="16">
-      <c r="A6" s="16" t="s">
+      <c r="B10" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.399999999999999">
+      <c r="A11" s="16" t="s">
         <v>565</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="16">
-      <c r="A7" s="16" t="s">
+      <c r="B11" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>638</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="17.399999999999999">
+      <c r="A12" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>505</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="16" t="s">
+      <c r="B12" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.399999999999999">
+      <c r="A13" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>594</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="16" t="s">
+      <c r="B13" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="15" customFormat="1" ht="17.399999999999999">
+      <c r="A14" s="15" t="s">
         <v>568</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>595</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="16" t="s">
-        <v>569</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>596</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="16" t="s">
-        <v>570</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>597</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="16">
-      <c r="A12" s="16" t="s">
-        <v>571</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="16" t="s">
-        <v>572</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="16" t="s">
-        <v>573</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="16">
-      <c r="B18" s="5" t="s">
-        <v>506</v>
-      </c>
+      <c r="C14" s="15" t="s">
+        <v>589</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17.399999999999999">
+      <c r="A15" s="16" t="s">
+        <v>653</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17.399999999999999">
+      <c r="A16" s="16" t="s">
+        <v>657</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="D16" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="17.399999999999999">
+      <c r="B18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5385,33 +5456,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5420,156 +5491,156 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" thickTop="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999">
+      <c r="A5" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.399999999999999">
+      <c r="A6" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16">
-      <c r="A5" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.399999999999999">
+      <c r="A7" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.399999999999999">
+      <c r="A8" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>634</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.399999999999999">
+      <c r="A9" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>633</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>635</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>636</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>452</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" s="13" customFormat="1">
       <c r="A10" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>624</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>631</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>638</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1">
       <c r="A11" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>625</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.399999999999999">
+      <c r="A12" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.399999999999999">
+      <c r="A13" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>639</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16">
-      <c r="A12" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>628</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="5" t="s">
-        <v>362</v>
-      </c>
       <c r="B13" s="5" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B14" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="C14" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="13" customFormat="1">
       <c r="A15" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started removing redundancy, moving properties
And making the ontology consistent. Also, fixing some domains to beable
to show them in the wiki
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1994,9 +1994,6 @@
     <t>Describing the cohorts a person is an imaging data collector of</t>
   </si>
   <si>
-    <t>Project,AcademicArticle, dcterms:contributor, author, Person</t>
-  </si>
-  <si>
     <t>Project,AcademicArticle,firstDraftContributor, Person</t>
   </si>
   <si>
@@ -2031,6 +2028,9 @@
   </si>
   <si>
     <t>Who contributed to writing a paper, or a project?</t>
+  </si>
+  <si>
+    <t>Project,AcademicArticle, contributor, author, Person</t>
   </si>
 </sst>
 </file>
@@ -3881,7 +3881,7 @@
         <v>124</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -4470,7 +4470,7 @@
         <v>542</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -4582,7 +4582,7 @@
         <v>132</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -5244,7 +5244,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -5286,10 +5286,10 @@
         <v>499</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>658</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>659</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>647</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -5313,7 +5313,7 @@
         <v>501</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -5325,7 +5325,7 @@
         <v>502</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -5410,12 +5410,12 @@
         <v>589</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.399999999999999">
       <c r="A15" s="16" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>224</v>
@@ -5426,19 +5426,24 @@
     </row>
     <row r="16" spans="1:4" ht="17.399999999999999">
       <c r="A16" s="16" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>654</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" t="s">
         <v>655</v>
       </c>
-      <c r="D16" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="17.399999999999999">
+    </row>
+    <row r="17" spans="1:3" ht="17.399999999999999">
+      <c r="A17" s="16"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" ht="17.399999999999999">
       <c r="B18" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed prop inconsistencies across ontology and added kind obj prop
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="16056" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="661">
   <si>
     <t>Requirement</t>
   </si>
@@ -596,9 +591,6 @@
     <t>Cohort, hasNumberOfParticipants, [positive integer]</t>
   </si>
   <si>
-    <t>Cohort, hasStatus, {"gathering participants" , "protocol preparation" , "published" , "revision"}</t>
-  </si>
-  <si>
     <t>Cohort, hasStudyDesign, {"Case-Control" , "Population-Based"}</t>
   </si>
   <si>
@@ -653,9 +645,6 @@
     <t>Describing the zip or postal code of an organization</t>
   </si>
   <si>
-    <t>Describing the type of an organization</t>
-  </si>
-  <si>
     <t>Person Ontology Requirements</t>
   </si>
   <si>
@@ -1419,9 +1408,6 @@
   </si>
   <si>
     <t>Organization, vcard:hasAddress, vcard:postalCode, [string]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization, rdf:type, {"College" ,"Center", "Consortium" , "Hospital" , "Institute" , "University", "Department"} </t>
   </si>
   <si>
     <t>SEE also O10</t>
@@ -1817,9 +1803,6 @@
     <t>WorkingGroup, shortName, [string]</t>
   </si>
   <si>
-    <t>WorkingGroup, rdf:type, [HealthyVariation,  GeneticStudy, Methodology, ClinicalPopulation]</t>
-  </si>
-  <si>
     <t>Project,hasDeveloper, Person</t>
   </si>
   <si>
@@ -2031,19 +2014,33 @@
   </si>
   <si>
     <t>Project,AcademicArticle, contributor, author, Person</t>
+  </si>
+  <si>
+    <t>Renamed to hasCohortStatus to avoid conflict with hasStatus from Person</t>
+  </si>
+  <si>
+    <t>Cohort, hasCohortStatus, {"gathering participants" , "protocol preparation" , "published" , "revision"}</t>
+  </si>
+  <si>
+    <t>WorkingGroup, kind, [string]</t>
+  </si>
+  <si>
+    <t>Describing the type of an organization  {"College" ,"Center", "Consortium" , "Hospital" , "Institute" , "University", "Department"}</t>
+  </si>
+  <si>
+    <t>Organization, kind, [string]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2786,34 +2783,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.796875" customWidth="1"/>
+    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="22.8">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -2822,12 +2819,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A5" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -2836,9 +2833,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>22</v>
@@ -2847,9 +2844,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -2858,9 +2855,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>14</v>
@@ -2869,9 +2866,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
@@ -2880,9 +2877,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>13</v>
@@ -2891,9 +2888,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>17</v>
@@ -2902,9 +2899,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>19</v>
@@ -2913,9 +2910,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
@@ -2924,9 +2921,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>25</v>
@@ -2935,9 +2932,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+    <row r="15" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A15" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>27</v>
@@ -2946,12 +2943,12 @@
         <v>28</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A16" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>29</v>
@@ -2960,9 +2957,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+    <row r="17" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A17" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>31</v>
@@ -2971,9 +2968,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
@@ -2982,9 +2979,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>35</v>
@@ -2993,9 +2990,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>37</v>
@@ -3004,23 +3001,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="10" customFormat="1" ht="17.399999999999999">
+    <row r="21" spans="1:4" s="10" customFormat="1" ht="16">
       <c r="A21" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>40</v>
@@ -3029,20 +3026,20 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>46</v>
@@ -3051,9 +3048,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>47</v>
@@ -3062,9 +3059,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>48</v>
@@ -3073,9 +3070,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
@@ -3084,9 +3081,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+    <row r="28" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A28" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>52</v>
@@ -3095,12 +3092,12 @@
         <v>53</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -3109,9 +3106,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A30" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>56</v>
@@ -3120,9 +3117,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+    <row r="31" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A31" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>58</v>
@@ -3131,12 +3128,12 @@
         <v>3</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>59</v>
@@ -3145,9 +3142,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>61</v>
@@ -3156,9 +3153,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A34" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>63</v>
@@ -3167,9 +3164,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>65</v>
@@ -3178,20 +3175,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A37" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>67</v>
@@ -3200,12 +3197,12 @@
         <v>68</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="16">
       <c r="A38" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>69</v>
@@ -3214,12 +3211,12 @@
         <v>70</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>71</v>
@@ -3228,12 +3225,12 @@
         <v>72</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>73</v>
@@ -3242,12 +3239,12 @@
         <v>74</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A41" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>75</v>
@@ -3256,12 +3253,12 @@
         <v>160</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A42" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>76</v>
@@ -3270,12 +3267,12 @@
         <v>161</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="9" customFormat="1" ht="17.399999999999999">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1" ht="16">
       <c r="A43" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>77</v>
@@ -3284,50 +3281,50 @@
         <v>162</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A45" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A46" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="B46" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A45" s="5" t="s">
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A47" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A46" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="D46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A47" s="5" t="s">
-        <v>306</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>78</v>
@@ -3336,9 +3333,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A48" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>79</v>
@@ -3347,9 +3344,9 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="49" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>80</v>
@@ -3358,9 +3355,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="50" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A50" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>81</v>
@@ -3369,9 +3366,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="51" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A51" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>82</v>
@@ -3380,9 +3377,9 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="52" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A52" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>83</v>
@@ -3391,9 +3388,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="53" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A53" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>84</v>
@@ -3402,9 +3399,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="54" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A54" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>85</v>
@@ -3413,9 +3410,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="55" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A55" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>86</v>
@@ -3424,9 +3421,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="56" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A56" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>87</v>
@@ -3435,9 +3432,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="57" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A57" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>88</v>
@@ -3446,9 +3443,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="58" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A58" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>89</v>
@@ -3457,9 +3454,9 @@
         <v>179</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="59" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A59" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>90</v>
@@ -3468,9 +3465,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="60" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A60" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>91</v>
@@ -3479,9 +3476,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A61" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>92</v>
@@ -3490,9 +3487,9 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="62" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A62" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>93</v>
@@ -3501,9 +3498,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A63" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>94</v>
@@ -3512,9 +3509,9 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A64" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>95</v>
@@ -3523,9 +3520,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="65" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A65" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>96</v>
@@ -3534,9 +3531,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="66" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A66" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>97</v>
@@ -3545,9 +3542,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="67" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A67" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>98</v>
@@ -3556,9 +3553,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="68" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A68" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>99</v>
@@ -3567,31 +3564,34 @@
         <v>168</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="69" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A69" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>657</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A70" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A71" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>102</v>
@@ -3600,9 +3600,9 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="72" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A72" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>103</v>
@@ -3611,9 +3611,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="73" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A73" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>104</v>
@@ -3622,9 +3622,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="74" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A74" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>105</v>
@@ -3633,9 +3633,9 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="75" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A75" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>106</v>
@@ -3644,105 +3644,105 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="76" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A76" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A77" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>108</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A78" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A79" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A80" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A81" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>112</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A82" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="B83" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="17.399999999999999">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16">
       <c r="B84" s="5" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="17.399999999999999">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16">
       <c r="B85" s="5" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -3760,27 +3760,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -3789,12 +3789,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>4</v>
@@ -3803,34 +3803,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>115</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>116</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>117</v>
@@ -3839,12 +3839,12 @@
         <v>118</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>119</v>
@@ -3853,12 +3853,12 @@
         <v>120</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>121</v>
@@ -3867,12 +3867,12 @@
         <v>122</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>123</v>
@@ -3881,12 +3881,12 @@
         <v>124</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>125</v>
@@ -3895,12 +3895,12 @@
         <v>126</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>127</v>
@@ -3909,12 +3909,12 @@
         <v>128</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>129</v>
@@ -3923,12 +3923,12 @@
         <v>130</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>131</v>
@@ -3937,9 +3937,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A15" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>133</v>
@@ -3948,9 +3948,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A16" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>135</v>
@@ -3959,9 +3959,9 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A17" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>137</v>
@@ -3970,9 +3970,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>139</v>
@@ -3981,12 +3981,12 @@
         <v>140</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>142</v>
@@ -3995,9 +3995,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>143</v>
@@ -4006,9 +4006,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A21" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>145</v>
@@ -4017,9 +4017,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>146</v>
@@ -4028,12 +4028,12 @@
         <v>147</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>148</v>
@@ -4042,23 +4042,23 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>150</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>151</v>
@@ -4067,23 +4067,23 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>152</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>153</v>
@@ -4092,9 +4092,9 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A28" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>155</v>
@@ -4103,137 +4103,137 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17.399999999999999">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16">
       <c r="A30" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16">
+      <c r="A31" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A32" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>603</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16">
+      <c r="A33" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17.399999999999999">
-      <c r="A31" s="16" t="s">
+      <c r="B33" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16">
+      <c r="A34" s="16" t="s">
         <v>575</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>504</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A32" s="5" t="s">
+      <c r="B34" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>600</v>
+      </c>
+      <c r="D34" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16">
+      <c r="A35" s="16" t="s">
         <v>576</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C35" s="5" t="s">
+        <v>588</v>
+      </c>
+      <c r="D35" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16">
+      <c r="A36" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16">
+      <c r="A37" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16">
+      <c r="A38" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>605</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16">
+      <c r="A39" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>591</v>
+      </c>
+      <c r="C39" s="16" t="s">
         <v>606</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17.399999999999999">
-      <c r="A33" s="16" t="s">
-        <v>577</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>512</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.399999999999999">
-      <c r="A34" s="16" t="s">
-        <v>578</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>604</v>
-      </c>
-      <c r="D34" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17.399999999999999">
-      <c r="A35" s="16" t="s">
-        <v>579</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>514</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="D35" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17.399999999999999">
-      <c r="A36" s="16" t="s">
-        <v>580</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>515</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17.399999999999999">
-      <c r="A37" s="16" t="s">
-        <v>581</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17.399999999999999">
-      <c r="A38" s="16" t="s">
-        <v>582</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17.399999999999999">
-      <c r="A39" s="16" t="s">
-        <v>583</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>595</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -4252,26 +4252,26 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4280,137 +4280,137 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A5" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A6" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A7" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="D5" s="5" t="s">
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A9" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A10" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A11" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>464</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A6" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A7" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A8" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A9" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A10" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A11" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A12" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A13" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A14" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -4428,26 +4428,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="B24" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.296875" customWidth="1"/>
-    <col min="3" max="3" width="77.296875" customWidth="1"/>
-    <col min="4" max="4" width="26.69921875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.33203125" customWidth="1"/>
+    <col min="3" max="3" width="77.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4456,597 +4456,597 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+      <c r="A4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A5" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
-      <c r="A4" s="5" t="s">
+      <c r="C5" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A6" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>542</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A5" s="5" t="s">
+      <c r="B6" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A7" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A6" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="B7" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D7" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A7" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D8" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A9" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A8" s="5" t="s">
+      <c r="C9" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A10" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B10" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A9" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A11" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="B11" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A10" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A11" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A12" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>132</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A15" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A16" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A14" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>543</v>
-      </c>
-      <c r="D14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A15" s="5" t="s">
+      <c r="C16" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A17" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A16" s="5" t="s">
+      <c r="B17" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A18" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A17" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>571</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A18" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>397</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D21" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A22" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>483</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A23" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="C21" s="15" t="s">
+      <c r="B23" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D21" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A22" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A24" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B24" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>486</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A23" s="5" t="s">
+      <c r="C24" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A25" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A24" s="5" t="s">
+      <c r="C25" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A26" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A25" s="5" t="s">
+      <c r="C26" s="16" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A27" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A26" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A27" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>240</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>404</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A29" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A30" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C28" s="15" t="s">
+      <c r="B30" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C30" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A31" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A32" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A29" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C29" s="5" t="s">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A33" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A34" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A35" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A30" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A31" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A32" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>488</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A33" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A34" s="5" t="s">
+      <c r="C35" s="16" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A36" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A37" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A38" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A39" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A40" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A41" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A42" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A43" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A44" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A45" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A46" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="C34" s="5" t="s">
+    </row>
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A47" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A48" s="5" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A35" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A36" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A37" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A38" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="C38" s="16" t="s">
+      <c r="B48" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C48" s="16" t="s">
         <v>550</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A39" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>551</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A40" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A41" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A42" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A43" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A44" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A45" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>613</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A46" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A47" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A48" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    </row>
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="17.399999999999999">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="16">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="17.399999999999999">
+    <row r="51" spans="1:4" ht="16">
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="17.399999999999999">
+    <row r="52" spans="1:4" ht="16">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="17.399999999999999">
+    <row r="53" spans="1:4" ht="16">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="17.399999999999999">
+    <row r="54" spans="1:4" ht="16">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="17.399999999999999">
+    <row r="55" spans="1:4" ht="16">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="17.399999999999999">
+    <row r="56" spans="1:4" ht="16">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="17.399999999999999">
+    <row r="57" spans="1:4" ht="16">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="17.399999999999999">
+    <row r="58" spans="1:4" ht="16">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="17.399999999999999">
+    <row r="59" spans="1:4" ht="16">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="17.399999999999999">
+    <row r="60" spans="1:4" ht="16">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
@@ -5064,25 +5064,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5091,142 +5091,142 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A9" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A10" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A8" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="C10" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A11" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A13" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+      <c r="A14" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="11" customFormat="1" ht="16">
+      <c r="A15" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A9" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A10" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A11" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A12" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>505</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A13" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
-      <c r="A14" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
-      <c r="A15" s="11" t="s">
-        <v>492</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>496</v>
-      </c>
       <c r="D15" s="11" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -5243,33 +5243,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="59.19921875" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5278,172 +5278,172 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>654</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A5" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A6" s="16" t="s">
+        <v>557</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="16">
+      <c r="A7" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>658</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>659</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
-      <c r="A5" s="16" t="s">
+      <c r="C7" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="16" t="s">
         <v>559</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>500</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>590</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
-      <c r="A6" s="16" t="s">
+      <c r="B8" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="16" t="s">
         <v>560</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>501</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>647</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="17.399999999999999">
-      <c r="A7" s="16" t="s">
+      <c r="B9" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="16" t="s">
         <v>561</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>502</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="B10" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>633</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>634</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="15" customFormat="1" ht="16">
+      <c r="A14" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>585</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="16" t="s">
         <v>648</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999">
-      <c r="A8" s="16" t="s">
-        <v>562</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>641</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>635</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999">
-      <c r="A9" s="16" t="s">
-        <v>563</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>636</v>
-      </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="17.399999999999999">
-      <c r="A10" s="16" t="s">
-        <v>564</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>637</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="17.399999999999999">
-      <c r="A11" s="16" t="s">
-        <v>565</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>638</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999">
-      <c r="A12" s="16" t="s">
-        <v>566</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>645</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.399999999999999">
-      <c r="A13" s="16" t="s">
-        <v>567</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="15" customFormat="1" ht="17.399999999999999">
-      <c r="A14" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>589</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17.399999999999999">
-      <c r="A15" s="16" t="s">
-        <v>652</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.399999999999999">
+    <row r="16" spans="1:4" ht="16">
       <c r="A16" s="16" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="D16" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17.399999999999999">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16">
       <c r="A17" s="16"/>
       <c r="B17" s="5"/>
       <c r="C17" s="16"/>
     </row>
-    <row r="18" spans="1:3" ht="17.399999999999999">
+    <row r="18" spans="1:3" ht="16">
       <c r="B18" s="5"/>
     </row>
   </sheetData>
@@ -5462,32 +5462,32 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.8">
+    <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5496,156 +5496,156 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" thickTop="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16">
+      <c r="A5" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.399999999999999">
-      <c r="A5" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="17.399999999999999">
-      <c r="A6" s="5" t="s">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>619</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="17.399999999999999">
-      <c r="A7" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>621</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" ht="17.399999999999999">
-      <c r="A8" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="17.399999999999999">
-      <c r="A9" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>623</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" s="13" customFormat="1">
       <c r="A10" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1">
       <c r="A11" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>621</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>625</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.399999999999999">
-      <c r="A12" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.399999999999999">
-      <c r="A13" s="5" t="s">
-        <v>360</v>
-      </c>
       <c r="B13" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B14" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="C14" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="13" customFormat="1">
       <c r="A15" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed WG title prop
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1797,9 +1797,6 @@
     <t>WorkingGroup, hasBriefDescription, [string]</t>
   </si>
   <si>
-    <t>WorkingGroup, dcterms:title, [string literal]</t>
-  </si>
-  <si>
     <t>WorkingGroup, shortName, [string]</t>
   </si>
   <si>
@@ -2029,6 +2026,9 @@
   </si>
   <si>
     <t>Organization, kind, [string]</t>
+  </si>
+  <si>
+    <t>WorkingGroup, fullName, [string literal]</t>
   </si>
 </sst>
 </file>
@@ -3572,10 +3572,10 @@
         <v>100</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3881,7 +3881,7 @@
         <v>124</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
@@ -3981,7 +3981,7 @@
         <v>140</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4050,10 +4050,10 @@
         <v>150</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>596</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4075,10 +4075,10 @@
         <v>152</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4122,7 +4122,7 @@
         <v>500</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16">
@@ -4133,7 +4133,7 @@
         <v>501</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4144,10 +4144,10 @@
         <v>508</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
@@ -4158,7 +4158,7 @@
         <v>509</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
@@ -4169,10 +4169,10 @@
         <v>510</v>
       </c>
       <c r="C34" s="15" t="s">
+        <v>599</v>
+      </c>
+      <c r="D34" t="s">
         <v>600</v>
-      </c>
-      <c r="D34" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16">
@@ -4183,7 +4183,7 @@
         <v>511</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D35" t="s">
         <v>522</v>
@@ -4197,7 +4197,7 @@
         <v>512</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16">
@@ -4208,7 +4208,7 @@
         <v>513</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
@@ -4219,10 +4219,10 @@
         <v>514</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16">
@@ -4230,10 +4230,10 @@
         <v>580</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -4385,10 +4385,10 @@
         <v>383</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>659</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4470,7 +4470,7 @@
         <v>539</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4582,7 +4582,7 @@
         <v>132</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4660,7 +4660,7 @@
         <v>229</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
@@ -4671,7 +4671,7 @@
         <v>230</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -4962,7 +4962,7 @@
         <v>468</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>525</v>
@@ -5065,7 +5065,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5193,7 +5193,7 @@
         <v>502</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5204,7 +5204,7 @@
         <v>503</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>583</v>
+        <v>660</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
@@ -5215,7 +5215,7 @@
         <v>490</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="11" customFormat="1" ht="16">
@@ -5226,7 +5226,7 @@
         <v>493</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -5286,10 +5286,10 @@
         <v>496</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>653</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>654</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>655</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -5301,7 +5301,7 @@
         <v>497</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -5313,7 +5313,7 @@
         <v>498</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -5325,7 +5325,7 @@
         <v>499</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -5334,10 +5334,10 @@
         <v>559</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -5346,10 +5346,10 @@
         <v>560</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -5358,10 +5358,10 @@
         <v>561</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -5370,10 +5370,10 @@
         <v>562</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -5382,10 +5382,10 @@
         <v>563</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
@@ -5393,10 +5393,10 @@
         <v>564</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="15" customFormat="1" ht="16">
@@ -5407,15 +5407,15 @@
         <v>218</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16">
       <c r="A15" s="16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>222</v>
@@ -5426,16 +5426,16 @@
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="16" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>649</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" t="s">
         <v>650</v>
-      </c>
-      <c r="D16" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16">
@@ -5504,13 +5504,13 @@
         <v>350</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>443</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
@@ -5521,7 +5521,7 @@
         <v>444</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -5533,7 +5533,7 @@
         <v>445</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -5545,7 +5545,7 @@
         <v>446</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -5557,7 +5557,7 @@
         <v>447</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -5569,7 +5569,7 @@
         <v>448</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -5578,13 +5578,13 @@
         <v>355</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1">
@@ -5595,10 +5595,10 @@
         <v>449</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
@@ -5606,10 +5606,10 @@
         <v>357</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
@@ -5617,10 +5617,10 @@
         <v>358</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -5628,10 +5628,10 @@
         <v>359</v>
       </c>
       <c r="B14" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C14" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="13" customFormat="1">
@@ -5639,13 +5639,13 @@
         <v>360</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding cohortgroup csv template
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="718">
   <si>
     <t>Requirement</t>
   </si>
@@ -2190,6 +2190,18 @@
   </si>
   <si>
     <t xml:space="preserve">  IN THEIR COHORTGROUP DOCUMENT. SOME POTENTIALLY COULD BE USED FOR PROJECT COHORTS</t>
+  </si>
+  <si>
+    <t>C100</t>
+  </si>
+  <si>
+    <t>Describing the cohort groups that belong to a cohort</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>Ask Neda/Aggie how they want to represent this relationship</t>
   </si>
 </sst>
 </file>
@@ -2978,10 +2990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4049,7 +4061,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="16">
+    <row r="97" spans="1:4" ht="16">
       <c r="A97" s="5" t="s">
         <v>668</v>
       </c>
@@ -4060,7 +4072,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="16">
+    <row r="98" spans="1:4" ht="16">
       <c r="A98" s="5" t="s">
         <v>685</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="16">
+    <row r="99" spans="1:4" ht="16">
       <c r="A99" s="5" t="s">
         <v>690</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="16">
+    <row r="100" spans="1:4" ht="16">
       <c r="A100" s="5" t="s">
         <v>695</v>
       </c>
@@ -4093,7 +4105,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="101" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A101" s="5" t="s">
         <v>700</v>
       </c>
@@ -4104,7 +4116,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="102" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A102" s="5" t="s">
         <v>701</v>
       </c>
@@ -4115,7 +4127,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="103" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A103" s="5" t="s">
         <v>702</v>
       </c>
@@ -4126,7 +4138,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="16">
+    <row r="104" spans="1:4" ht="16">
       <c r="A104" s="5" t="s">
         <v>709</v>
       </c>
@@ -4135,6 +4147,20 @@
       </c>
       <c r="C104" s="5" t="s">
         <v>710</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" s="9" customFormat="1">
+      <c r="A105" s="9" t="s">
+        <v>714</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>715</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>717</v>
       </c>
     </row>
   </sheetData>
@@ -4152,7 +4178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated cohortgroup ont and csv
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="770">
   <si>
     <t>Requirement</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Describing the location of the data collection of a cohort</t>
-  </si>
-  <si>
-    <t>Cohort, hasLocationOfDataCollection, Location</t>
   </si>
   <si>
     <t>Describing the min and max values of the medical rating criteria</t>
@@ -2057,54 +2054,6 @@
     <t>C92</t>
   </si>
   <si>
-    <t>Describing the amount of T1-weighted image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfT1w, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>Describing the amount of electroencephalography image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of arterial spine labeling image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of total body fat measured on MRI image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of resting state fMRI image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of Susceptibility weighted imaging image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of T2 image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>Describing the amount of diffusion MRI image data collected by a cohort group</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfdMRI [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfT2, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfSWI, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfrsfMRI, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOftbfMRI, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfASL, [non-negative integer]</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasNumberOfEEG, [non-negative integer]</t>
-  </si>
-  <si>
     <t>C93</t>
   </si>
   <si>
@@ -2123,15 +2072,9 @@
     <t>C94</t>
   </si>
   <si>
-    <t>Describing the study feature of a cohort group (Clinical trial; Twin/Family study; Logitudinal; Retrospective hospital data)</t>
-  </si>
-  <si>
     <t>CohortGroup, hasStudyFeature, [string]</t>
   </si>
   <si>
-    <t>Describing the genetic data collected by a cohort group (genome-wide; whole genome; CNVs; exome; some SNPs; blood/saliva collected, DNA extracted, no genotyping; blood/saliva collected, no DNA extracted; epigenetics - blood; epigenetics - saliva; mitocondrial genotyping; plasma)</t>
-  </si>
-  <si>
     <t>CohortGroup, hasAgeGroup, [string]</t>
   </si>
   <si>
@@ -2141,9 +2084,6 @@
     <t>CohortGroup, hasAdditionalDemographic, [string]</t>
   </si>
   <si>
-    <t>Describing the additional demographics defining a cohort group (IQ; Handedness; ParentalSES; IndividualSES)</t>
-  </si>
-  <si>
     <t>CohortGroup, hasNumberOfMale, [non-negative integer]</t>
   </si>
   <si>
@@ -2202,6 +2142,222 @@
   </si>
   <si>
     <t>Ask Neda/Aggie how they want to represent this relationship</t>
+  </si>
+  <si>
+    <t>Cohort, hasCollectionSite, [string]</t>
+  </si>
+  <si>
+    <t>C101</t>
+  </si>
+  <si>
+    <t>Describing the species of the subjects of a cohort</t>
+  </si>
+  <si>
+    <t>Cohort, hasSpecies, [string]</t>
+  </si>
+  <si>
+    <t>Describing the amount of electroencephalography image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of arterial spine labeling image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of total body fat measured on MRI image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of resting state fMRI image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of Susceptibility weighted imaging image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of T2 image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of diffusion MRI image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>Describing the amount of T1-weighted image data collected by a project cohort</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfT1w, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfdMRI [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfT2, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfSWI, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfrsfMRI, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOftbfMRI, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfASL, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasNumberOfEEG, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>C102</t>
+  </si>
+  <si>
+    <t>Describing the types of brain structural/functional data collected by a cohort group (T1w; dMRI; T2w; SWI; rsfMRI; tbfMRI; ASL; EEG; MEG; Histology; CT; Head Circumference; Cognitive/Behavior assessments)</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasBrainStructuralData, [string]</t>
+  </si>
+  <si>
+    <t>Describing the study feature of a cohort group (Clinical trial; Twin/Family study; Logitudinal; in-vivo; ex-vivo; post-mortem)</t>
+  </si>
+  <si>
+    <t>C103</t>
+  </si>
+  <si>
+    <t>Describing the number of cis male individuals in a cohort group</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasNumberOfCisMale, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>C104</t>
+  </si>
+  <si>
+    <t>Describing the number of cis female individuals in a cohort group</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasNumberOfCisFemale, [non-negative integer]</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>C106</t>
+  </si>
+  <si>
+    <t>Describing the handedness criteria for individuals in a cohort group (RH only; LH only; matched; assessed but not used as selection criteria; not assessed)</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasHandedness, [string]</t>
+  </si>
+  <si>
+    <t>Describing the additional demographics defining a cohort group (Height; Weight; Ethnicity; IQ; ParentalSES; IndividualSES)</t>
+  </si>
+  <si>
+    <t>Describing the genetic data collected by a cohort group (MDD; Bipolar Disorder; Schizophrenia; OCD; ADHD; HIV; Autism; Addiction / SUD; Epilepsy; Anorexia / Eating Disorders; Parkinson; PTSD; Irritability; Stroke Recovery; Cerebellar Ataxia; Generalized anxiety; Panic disorder; Social anxiety; Early Onset Psychosis; Tourette's Syndrome; Brain Injury; Cancer &amp; Chemotherapy; Sleep; Suicidal Thoughts and Behaviors; Lysosome Storage Diseases; 22q DS; CNVs)</t>
+  </si>
+  <si>
+    <t>Removed to express each data type as an individual percent</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentGenomewideGenotyping, [double]</t>
+  </si>
+  <si>
+    <t>C107</t>
+  </si>
+  <si>
+    <t>C108</t>
+  </si>
+  <si>
+    <t>C109</t>
+  </si>
+  <si>
+    <t>C110</t>
+  </si>
+  <si>
+    <t>C111</t>
+  </si>
+  <si>
+    <t>C112</t>
+  </si>
+  <si>
+    <t>C113</t>
+  </si>
+  <si>
+    <t>C114</t>
+  </si>
+  <si>
+    <t>C115</t>
+  </si>
+  <si>
+    <t>C116</t>
+  </si>
+  <si>
+    <t>C117</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentWholeGenomeSequencing, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentExomeSequencing, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentSelectLoci, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentDNAExtractionNoGenotyping, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentBloodSalivaCollection, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentEpigeneticsBlood, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentEpigeneticsSaliva, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentMitochondrialGenotyping, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentPlasma, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentTranscriptomics, [double]</t>
+  </si>
+  <si>
+    <t>CohortGroup, hasPercentGeneExpression, [double]</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from genome-wide genotyping</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from whole genome sequencing</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from exome sequencing</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from select loci (some SNPs/CNVs)</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from DNA extraction with no genotyping</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from blood/saliva collected/stored with NO DNA extracted</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from mitochondrial genotyping</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from plasma</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from transcriptomics</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from gene expression</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from blood epigenetics</t>
+  </si>
+  <si>
+    <t>Describing the percent of cohort group biosamples which are from saliva epigenetics</t>
   </si>
 </sst>
 </file>
@@ -2363,7 +2519,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="132">
+  <cellStyleXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2496,8 +2652,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -2520,8 +2736,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="132">
+  <cellStyles count="192">
     <cellStyle name="Bad" xfId="59" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2588,6 +2805,36 @@
     <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2651,6 +2898,36 @@
     <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="60" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -2990,10 +3267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3008,18 +3285,18 @@
         <v>6</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>712</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22">
       <c r="B2" s="2"/>
       <c r="C2" s="9" t="s">
-        <v>713</v>
+        <v>693</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -3028,12 +3305,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="9" customFormat="1" ht="16" thickTop="1">
       <c r="A5" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>7</v>
@@ -3044,7 +3321,7 @@
     </row>
     <row r="6" spans="1:4" s="9" customFormat="1">
       <c r="A6" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>21</v>
@@ -3055,7 +3332,7 @@
     </row>
     <row r="7" spans="1:4" s="9" customFormat="1">
       <c r="A7" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>14</v>
@@ -3066,7 +3343,7 @@
     </row>
     <row r="8" spans="1:4" s="9" customFormat="1">
       <c r="A8" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>13</v>
@@ -3077,7 +3354,7 @@
     </row>
     <row r="9" spans="1:4" s="9" customFormat="1">
       <c r="A9" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>22</v>
@@ -3088,7 +3365,7 @@
     </row>
     <row r="10" spans="1:4" s="9" customFormat="1">
       <c r="A10" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>12</v>
@@ -3099,7 +3376,7 @@
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1">
       <c r="A11" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>16</v>
@@ -3110,7 +3387,7 @@
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1">
       <c r="A12" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>18</v>
@@ -3121,7 +3398,7 @@
     </row>
     <row r="13" spans="1:4" s="9" customFormat="1">
       <c r="A13" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>23</v>
@@ -3132,7 +3409,7 @@
     </row>
     <row r="14" spans="1:4" s="9" customFormat="1">
       <c r="A14" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>24</v>
@@ -3143,7 +3420,7 @@
     </row>
     <row r="15" spans="1:4" s="7" customFormat="1" ht="16">
       <c r="A15" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>26</v>
@@ -3154,7 +3431,7 @@
     </row>
     <row r="16" spans="1:4" s="7" customFormat="1" ht="16">
       <c r="A16" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>28</v>
@@ -3165,7 +3442,7 @@
     </row>
     <row r="17" spans="1:3" s="7" customFormat="1" ht="16">
       <c r="A17" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>30</v>
@@ -3176,7 +3453,7 @@
     </row>
     <row r="18" spans="1:3" s="9" customFormat="1">
       <c r="A18" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>32</v>
@@ -3187,7 +3464,7 @@
     </row>
     <row r="19" spans="1:3" s="9" customFormat="1">
       <c r="A19" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>34</v>
@@ -3198,7 +3475,7 @@
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>36</v>
@@ -3209,18 +3486,18 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="9" customFormat="1">
       <c r="A22" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>39</v>
@@ -3231,18 +3508,18 @@
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1">
       <c r="A23" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="9" customFormat="1">
       <c r="A24" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>45</v>
@@ -3253,7 +3530,7 @@
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>46</v>
@@ -3262,111 +3539,111 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="9" customFormat="1">
-      <c r="A26" s="9" t="s">
-        <v>276</v>
-      </c>
-      <c r="B26" s="9" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>275</v>
+      </c>
+      <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>48</v>
+      <c r="C26" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1">
       <c r="A27" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="9" customFormat="1">
       <c r="A28" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="9" customFormat="1">
       <c r="A29" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="9" customFormat="1">
       <c r="A30" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="9" customFormat="1">
       <c r="A32" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="9" customFormat="1">
       <c r="A34" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>2</v>
@@ -3374,793 +3651,983 @@
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="9" customFormat="1">
       <c r="A37" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="9" customFormat="1">
       <c r="A38" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>69</v>
-      </c>
       <c r="D38" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="9" customFormat="1">
       <c r="A39" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>71</v>
-      </c>
       <c r="D39" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="9" customFormat="1">
       <c r="A40" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="7" customFormat="1" ht="16">
       <c r="A41" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="7" customFormat="1" ht="16">
       <c r="A42" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="7" customFormat="1" ht="16">
       <c r="A43" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="9" customFormat="1">
       <c r="A44" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="9" customFormat="1">
       <c r="A45" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="9" customFormat="1">
       <c r="A46" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1">
       <c r="A47" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1">
       <c r="A48" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1">
       <c r="A49" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="9" customFormat="1">
       <c r="A50" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>694</v>
+        <v>675</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="9" customFormat="1">
       <c r="A52" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="9" customFormat="1">
       <c r="A55" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:3" s="9" customFormat="1">
       <c r="A56" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1">
       <c r="A57" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:3" s="9" customFormat="1">
       <c r="A58" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="9" customFormat="1">
       <c r="A59" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="9" customFormat="1">
       <c r="A60" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1">
       <c r="A61" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="9" customFormat="1">
       <c r="A62" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="9" customFormat="1">
       <c r="A63" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
       <c r="A64" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>699</v>
+        <v>679</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A65" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>698</v>
+        <v>678</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A66" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A67" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="9" customFormat="1">
       <c r="A68" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A69" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A70" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="9" customFormat="1">
       <c r="A71" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="9" customFormat="1">
       <c r="A72" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="9" customFormat="1">
       <c r="A73" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="9" customFormat="1">
       <c r="A74" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="9" customFormat="1">
       <c r="A75" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="9" customFormat="1">
       <c r="A76" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="9" customFormat="1">
       <c r="A77" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="9" customFormat="1">
       <c r="A78" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="9" customFormat="1">
       <c r="A79" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="9" customFormat="1">
       <c r="A80" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="9" customFormat="1">
       <c r="A81" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="9" customFormat="1">
       <c r="A82" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="10" customFormat="1">
       <c r="A83" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="10" customFormat="1">
       <c r="A84" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="10" customFormat="1">
       <c r="A85" s="10" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B85" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="C85" s="10" t="s">
         <v>498</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="16">
       <c r="A86" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>647</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A87" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="C87" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>653</v>
-      </c>
       <c r="D87" s="13" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="16">
       <c r="A88" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="C88" t="s">
         <v>655</v>
-      </c>
-      <c r="C88" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="10" customFormat="1">
       <c r="A89" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="B89" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="C89" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="D89" s="10" t="s">
         <v>659</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="16">
       <c r="A90" s="5" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>671</v>
+        <v>702</v>
       </c>
       <c r="C90" t="s">
-        <v>684</v>
+        <v>717</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="16">
       <c r="A91" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>672</v>
+        <v>703</v>
       </c>
       <c r="C91" t="s">
-        <v>683</v>
+        <v>716</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="16">
       <c r="A92" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>673</v>
+        <v>704</v>
       </c>
       <c r="C92" t="s">
-        <v>682</v>
+        <v>715</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="16">
       <c r="A93" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>674</v>
+        <v>705</v>
       </c>
       <c r="C93" t="s">
-        <v>681</v>
+        <v>714</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="16">
       <c r="A94" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>675</v>
+        <v>706</v>
       </c>
       <c r="C94" t="s">
-        <v>680</v>
+        <v>713</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="16">
       <c r="A95" s="5" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>676</v>
+        <v>707</v>
       </c>
       <c r="C95" t="s">
-        <v>679</v>
+        <v>712</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="16">
       <c r="A96" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>677</v>
+        <v>708</v>
       </c>
       <c r="C96" t="s">
-        <v>678</v>
+        <v>711</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="16">
       <c r="A97" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="C97" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="12" customFormat="1" ht="16">
+      <c r="A98" s="11" t="s">
         <v>668</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B98" s="11" t="s">
+        <v>733</v>
+      </c>
+      <c r="C98" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="C97" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="16">
-      <c r="A98" s="5" t="s">
-        <v>685</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>693</v>
-      </c>
-      <c r="C98" t="s">
-        <v>686</v>
+      <c r="D98" s="14" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="16">
       <c r="A99" s="5" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>691</v>
+        <v>721</v>
       </c>
       <c r="C99" t="s">
-        <v>692</v>
+        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="16">
       <c r="A100" s="5" t="s">
-        <v>695</v>
+        <v>676</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>697</v>
+        <v>732</v>
       </c>
       <c r="C100" t="s">
-        <v>696</v>
+        <v>677</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A101" s="5" t="s">
-        <v>700</v>
+        <v>680</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>706</v>
+        <v>686</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>708</v>
+        <v>688</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A102" s="5" t="s">
-        <v>701</v>
+        <v>681</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>705</v>
+        <v>685</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>703</v>
+        <v>683</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A103" s="5" t="s">
-        <v>702</v>
+        <v>682</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>707</v>
+        <v>687</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>704</v>
+        <v>684</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="16">
       <c r="A104" s="5" t="s">
-        <v>709</v>
+        <v>689</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>711</v>
+        <v>691</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>710</v>
+        <v>690</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="9" customFormat="1">
       <c r="A105" s="9" t="s">
-        <v>714</v>
+        <v>694</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>715</v>
+        <v>695</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>716</v>
+        <v>696</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>717</v>
+        <v>697</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="16">
+      <c r="A106" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="16">
+      <c r="A107" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B107" t="s">
+        <v>719</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="16">
+      <c r="A108" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>723</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="16">
+      <c r="A109" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="16">
+      <c r="A110" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="16">
+      <c r="A111" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="16">
+      <c r="A112" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="16">
+      <c r="A113" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="16">
+      <c r="A114" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="16">
+      <c r="A115" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="C115" s="5" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="16">
+      <c r="A116" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="16">
+      <c r="A117" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="16">
+      <c r="A118" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="16">
+      <c r="A119" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="16">
+      <c r="A120" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="16">
+      <c r="A121" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="16">
+      <c r="A122" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>757</v>
       </c>
     </row>
   </sheetData>
@@ -4190,15 +4657,15 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4207,12 +4674,12 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -4223,213 +4690,213 @@
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>116</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>118</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>120</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="D10" s="13" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>124</v>
-      </c>
       <c r="D11" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>126</v>
-      </c>
       <c r="D12" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="D13" s="13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A15" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A16" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A17" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>138</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>141</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A21" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
@@ -4437,221 +4904,221 @@
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>576</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>577</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>578</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A28" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16">
       <c r="A30" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16">
       <c r="A31" s="13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16">
       <c r="A33" s="13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16">
       <c r="A34" s="13" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C34" s="12" t="s">
+        <v>579</v>
+      </c>
+      <c r="D34" t="s">
         <v>580</v>
-      </c>
-      <c r="D34" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16">
       <c r="A35" s="13" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D35" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16">
       <c r="A36" s="13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16">
       <c r="A37" s="13" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16">
       <c r="A38" s="13" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16">
       <c r="A39" s="13" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
@@ -4681,15 +5148,15 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4698,137 +5165,137 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>635</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>419</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -4860,12 +5327,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -4874,197 +5341,197 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>203</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>205</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A15" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A16" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A17" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B17" s="13" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>550</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A18" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>44</v>
@@ -5072,365 +5539,365 @@
     </row>
     <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A19" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A20" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>225</v>
-      </c>
       <c r="D21" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A22" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A23" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A24" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A25" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A26" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A27" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>233</v>
-      </c>
       <c r="D28" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A29" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A30" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A31" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A32" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A33" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A34" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>461</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A35" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A36" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A37" s="5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A38" s="5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A39" s="5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A40" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A41" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A42" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A43" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A44" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A45" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A46" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A47" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A48" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A49" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C49" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>508</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16">
@@ -5495,12 +5962,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5509,26 +5976,26 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A5" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -5536,115 +6003,115 @@
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A6" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A7" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A8" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A9" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A10" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>251</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A11" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A12" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A13" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A14" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="8" customFormat="1" ht="16">
       <c r="A15" s="8" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>
@@ -5674,20 +6141,20 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5696,164 +6163,164 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="13" customFormat="1" ht="17" thickTop="1">
       <c r="A4" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>629</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>630</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>631</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" s="13" customFormat="1" ht="16">
       <c r="A5" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" s="13" customFormat="1" ht="16">
       <c r="A6" s="13" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" ht="16">
       <c r="A7" s="13" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="16">
       <c r="A8" s="13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="16">
       <c r="A9" s="13" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="16">
       <c r="A10" s="13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="16">
       <c r="A11" s="13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="12" customFormat="1" ht="16">
       <c r="A14" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16">
       <c r="A15" s="13" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
       <c r="A16" s="13" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>625</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" t="s">
         <v>626</v>
-      </c>
-      <c r="D16" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16">
@@ -5892,20 +6359,20 @@
   <sheetData>
     <row r="1" spans="1:4" ht="22">
       <c r="B1" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19" thickBot="1">
       <c r="A3" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -5914,156 +6381,156 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="10" customFormat="1" ht="16" thickTop="1">
       <c r="A4" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16">
       <c r="A7" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="16">
       <c r="A8" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="16">
       <c r="A9" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" s="10" customFormat="1">
       <c r="A10" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="10" customFormat="1">
       <c r="A11" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
       <c r="A12" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16">
       <c r="A13" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B14" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C14" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="10" customFormat="1">
       <c r="A15" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated reqs and dataset schema
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dgarijo\Documents\GitHub\EnigmaOntology\requirements\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort Ontology" sheetId="2" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <sheet name="Role Ontology" sheetId="10" r:id="rId6"/>
     <sheet name="Protocol Ontology" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="779">
   <si>
     <t>Requirement</t>
   </si>
@@ -2386,12 +2391,33 @@
   <si>
     <t>Pr37</t>
   </si>
+  <si>
+    <t>What are the datasets associated to a project cohort? (There may be more than one)</t>
+  </si>
+  <si>
+    <t>C118</t>
+  </si>
+  <si>
+    <t>C119</t>
+  </si>
+  <si>
+    <t>What are the statistics associated to a project cohort?</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasDataset, Dataset</t>
+  </si>
+  <si>
+    <t>ProjectCohort, hasStatistics, Dataset</t>
+  </si>
+  <si>
+    <t>All the dataset metadata is captured with schema.org</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3307,20 +3333,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="C110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="113" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="90.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3328,13 +3354,13 @@
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22">
+    <row r="2" spans="1:4" ht="22.8">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19" thickBot="1">
+    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>253</v>
       </c>
@@ -3348,7 +3374,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="16" thickTop="1">
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="16.2" thickTop="1">
       <c r="A5" s="8" t="s">
         <v>254</v>
       </c>
@@ -3458,7 +3484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="7" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A15" s="7" t="s">
         <v>264</v>
       </c>
@@ -3469,7 +3495,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="7" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A16" s="7" t="s">
         <v>265</v>
       </c>
@@ -3480,7 +3506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="7" customFormat="1" ht="16">
+    <row r="17" spans="1:3" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A17" s="7" t="s">
         <v>266</v>
       </c>
@@ -3568,7 +3594,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="25" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A25" s="5" t="s">
         <v>274</v>
       </c>
@@ -3656,7 +3682,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A33" s="5" t="s">
         <v>282</v>
       </c>
@@ -3678,7 +3704,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A35" s="5" t="s">
         <v>284</v>
       </c>
@@ -3689,7 +3715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A36" s="5" t="s">
         <v>285</v>
       </c>
@@ -3753,7 +3779,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="7" customFormat="1" ht="16">
+    <row r="41" spans="1:4" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A41" s="7" t="s">
         <v>290</v>
       </c>
@@ -3764,7 +3790,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="7" customFormat="1" ht="16">
+    <row r="42" spans="1:4" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A42" s="7" t="s">
         <v>291</v>
       </c>
@@ -3775,7 +3801,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="7" customFormat="1" ht="16">
+    <row r="43" spans="1:4" s="7" customFormat="1" ht="17.399999999999999">
       <c r="A43" s="7" t="s">
         <v>292</v>
       </c>
@@ -4006,7 +4032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="5" customFormat="1" ht="16">
+    <row r="64" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A64" s="5" t="s">
         <v>313</v>
       </c>
@@ -4017,7 +4043,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="65" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A65" s="5" t="s">
         <v>314</v>
       </c>
@@ -4028,7 +4054,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="66" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A66" s="5" t="s">
         <v>315</v>
       </c>
@@ -4039,7 +4065,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="67" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A67" s="5" t="s">
         <v>316</v>
       </c>
@@ -4061,7 +4087,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="69" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A69" s="5" t="s">
         <v>318</v>
       </c>
@@ -4075,7 +4101,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="70" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="70" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A70" s="5" t="s">
         <v>319</v>
       </c>
@@ -4251,7 +4277,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="16">
+    <row r="86" spans="1:4" ht="17.399999999999999">
       <c r="A86" s="5" t="s">
         <v>638</v>
       </c>
@@ -4262,7 +4288,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="87" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A87" s="5" t="s">
         <v>643</v>
       </c>
@@ -4276,7 +4302,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16">
+    <row r="88" spans="1:4" ht="17.399999999999999">
       <c r="A88" s="5" t="s">
         <v>646</v>
       </c>
@@ -4301,7 +4327,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="16">
+    <row r="90" spans="1:4" ht="17.399999999999999">
       <c r="A90" s="5" t="s">
         <v>653</v>
       </c>
@@ -4312,7 +4338,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16">
+    <row r="91" spans="1:4" ht="17.399999999999999">
       <c r="A91" s="5" t="s">
         <v>654</v>
       </c>
@@ -4323,7 +4349,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="16">
+    <row r="92" spans="1:4" ht="17.399999999999999">
       <c r="A92" s="5" t="s">
         <v>655</v>
       </c>
@@ -4334,7 +4360,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16">
+    <row r="93" spans="1:4" ht="17.399999999999999">
       <c r="A93" s="5" t="s">
         <v>656</v>
       </c>
@@ -4345,7 +4371,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16">
+    <row r="94" spans="1:4" ht="17.399999999999999">
       <c r="A94" s="5" t="s">
         <v>657</v>
       </c>
@@ -4356,7 +4382,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16">
+    <row r="95" spans="1:4" ht="17.399999999999999">
       <c r="A95" s="5" t="s">
         <v>658</v>
       </c>
@@ -4367,7 +4393,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16">
+    <row r="96" spans="1:4" ht="17.399999999999999">
       <c r="A96" s="5" t="s">
         <v>659</v>
       </c>
@@ -4378,7 +4404,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16">
+    <row r="97" spans="1:4" ht="17.399999999999999">
       <c r="A97" s="5" t="s">
         <v>660</v>
       </c>
@@ -4389,7 +4415,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="11" customFormat="1" ht="16">
+    <row r="98" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
       <c r="A98" s="10" t="s">
         <v>661</v>
       </c>
@@ -4403,7 +4429,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="16">
+    <row r="99" spans="1:4" ht="17.399999999999999">
       <c r="A99" s="5" t="s">
         <v>666</v>
       </c>
@@ -4414,7 +4440,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="16">
+    <row r="100" spans="1:4" ht="17.399999999999999">
       <c r="A100" s="5" t="s">
         <v>669</v>
       </c>
@@ -4425,7 +4451,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="101" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="101" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A101" s="5" t="s">
         <v>673</v>
       </c>
@@ -4436,7 +4462,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="102" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="102" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A102" s="5" t="s">
         <v>674</v>
       </c>
@@ -4447,7 +4473,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="103" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A103" s="5" t="s">
         <v>675</v>
       </c>
@@ -4458,7 +4484,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="16">
+    <row r="104" spans="1:4" ht="17.399999999999999">
       <c r="A104" s="5" t="s">
         <v>682</v>
       </c>
@@ -4483,7 +4509,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="16">
+    <row r="106" spans="1:4" ht="17.399999999999999">
       <c r="A106" s="5" t="s">
         <v>692</v>
       </c>
@@ -4494,7 +4520,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16">
+    <row r="107" spans="1:4" ht="17.399999999999999">
       <c r="A107" s="5" t="s">
         <v>711</v>
       </c>
@@ -4505,7 +4531,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16">
+    <row r="108" spans="1:4" ht="17.399999999999999">
       <c r="A108" s="5" t="s">
         <v>715</v>
       </c>
@@ -4516,7 +4542,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="16">
+    <row r="109" spans="1:4" ht="17.399999999999999">
       <c r="A109" s="5" t="s">
         <v>718</v>
       </c>
@@ -4527,7 +4553,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16">
+    <row r="110" spans="1:4" ht="17.399999999999999">
       <c r="A110" s="5" t="s">
         <v>721</v>
       </c>
@@ -4538,7 +4564,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16">
+    <row r="111" spans="1:4" ht="17.399999999999999">
       <c r="A111" s="5" t="s">
         <v>722</v>
       </c>
@@ -4549,7 +4575,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="16">
+    <row r="112" spans="1:4" ht="17.399999999999999">
       <c r="A112" s="5" t="s">
         <v>729</v>
       </c>
@@ -4560,7 +4586,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="16">
+    <row r="113" spans="1:4" ht="17.399999999999999">
       <c r="A113" s="5" t="s">
         <v>730</v>
       </c>
@@ -4571,7 +4597,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="16">
+    <row r="114" spans="1:4" ht="17.399999999999999">
       <c r="A114" s="5" t="s">
         <v>731</v>
       </c>
@@ -4582,7 +4608,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="16">
+    <row r="115" spans="1:4" ht="17.399999999999999">
       <c r="A115" s="5" t="s">
         <v>732</v>
       </c>
@@ -4593,7 +4619,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="16">
+    <row r="116" spans="1:4" ht="17.399999999999999">
       <c r="A116" s="5" t="s">
         <v>733</v>
       </c>
@@ -4604,7 +4630,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="16">
+    <row r="117" spans="1:4" ht="17.399999999999999">
       <c r="A117" s="5" t="s">
         <v>734</v>
       </c>
@@ -4615,7 +4641,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="16">
+    <row r="118" spans="1:4" ht="17.399999999999999">
       <c r="A118" s="5" t="s">
         <v>735</v>
       </c>
@@ -4626,7 +4652,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="16">
+    <row r="119" spans="1:4" ht="17.399999999999999">
       <c r="A119" s="5" t="s">
         <v>736</v>
       </c>
@@ -4637,7 +4663,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="16">
+    <row r="120" spans="1:4" ht="17.399999999999999">
       <c r="A120" s="5" t="s">
         <v>737</v>
       </c>
@@ -4648,7 +4674,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="16">
+    <row r="121" spans="1:4" ht="17.399999999999999">
       <c r="A121" s="5" t="s">
         <v>738</v>
       </c>
@@ -4659,7 +4685,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="16">
+    <row r="122" spans="1:4" ht="17.399999999999999">
       <c r="A122" s="5" t="s">
         <v>739</v>
       </c>
@@ -4668,6 +4694,31 @@
       </c>
       <c r="C122" s="5" t="s">
         <v>750</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="17.399999999999999">
+      <c r="A124" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="17.399999999999999">
+      <c r="A125" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>777</v>
       </c>
     </row>
   </sheetData>
@@ -4689,13 +4740,13 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>111</v>
       </c>
@@ -4703,7 +4754,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -4717,7 +4768,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>337</v>
       </c>
@@ -4728,7 +4779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
         <v>338</v>
       </c>
@@ -4742,7 +4793,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
         <v>339</v>
       </c>
@@ -4753,7 +4804,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
         <v>424</v>
       </c>
@@ -4767,7 +4818,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
         <v>340</v>
       </c>
@@ -4781,7 +4832,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
         <v>341</v>
       </c>
@@ -4795,7 +4846,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A10" s="5" t="s">
         <v>342</v>
       </c>
@@ -4809,7 +4860,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A11" s="5" t="s">
         <v>343</v>
       </c>
@@ -4823,7 +4874,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
         <v>344</v>
       </c>
@@ -4837,7 +4888,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
         <v>345</v>
       </c>
@@ -4851,7 +4902,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="5" t="s">
         <v>346</v>
       </c>
@@ -4862,7 +4913,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A15" s="5" t="s">
         <v>347</v>
       </c>
@@ -4873,7 +4924,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A16" s="5" t="s">
         <v>348</v>
       </c>
@@ -4884,7 +4935,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
         <v>349</v>
       </c>
@@ -4895,7 +4946,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A18" s="5" t="s">
         <v>350</v>
       </c>
@@ -4909,7 +4960,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A19" s="5" t="s">
         <v>351</v>
       </c>
@@ -4920,7 +4971,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A20" s="5" t="s">
         <v>352</v>
       </c>
@@ -4931,7 +4982,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A21" s="5" t="s">
         <v>353</v>
       </c>
@@ -4942,7 +4993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A22" s="5" t="s">
         <v>354</v>
       </c>
@@ -4956,7 +5007,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A23" s="5" t="s">
         <v>355</v>
       </c>
@@ -4967,7 +5018,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A24" s="5" t="s">
         <v>356</v>
       </c>
@@ -4981,7 +5032,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A25" s="5" t="s">
         <v>357</v>
       </c>
@@ -4992,7 +5043,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A26" s="5" t="s">
         <v>358</v>
       </c>
@@ -5006,7 +5057,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A27" s="5" t="s">
         <v>359</v>
       </c>
@@ -5017,7 +5068,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A28" s="5" t="s">
         <v>360</v>
       </c>
@@ -5028,7 +5079,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A29" s="5" t="s">
         <v>473</v>
       </c>
@@ -5039,7 +5090,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16">
+    <row r="30" spans="1:4" ht="17.399999999999999">
       <c r="A30" s="12" t="s">
         <v>548</v>
       </c>
@@ -5050,7 +5101,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16">
+    <row r="31" spans="1:4" ht="17.399999999999999">
       <c r="A31" s="12" t="s">
         <v>549</v>
       </c>
@@ -5061,7 +5112,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A32" s="5" t="s">
         <v>550</v>
       </c>
@@ -5075,7 +5126,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16">
+    <row r="33" spans="1:4" ht="17.399999999999999">
       <c r="A33" s="12" t="s">
         <v>551</v>
       </c>
@@ -5086,7 +5137,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16">
+    <row r="34" spans="1:4" ht="17.399999999999999">
       <c r="A34" s="12" t="s">
         <v>552</v>
       </c>
@@ -5100,7 +5151,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16">
+    <row r="35" spans="1:4" ht="17.399999999999999">
       <c r="A35" s="12" t="s">
         <v>553</v>
       </c>
@@ -5114,7 +5165,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="16">
+    <row r="36" spans="1:4" ht="17.399999999999999">
       <c r="A36" s="12" t="s">
         <v>554</v>
       </c>
@@ -5125,7 +5176,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16">
+    <row r="37" spans="1:4" ht="17.399999999999999">
       <c r="A37" s="12" t="s">
         <v>555</v>
       </c>
@@ -5136,7 +5187,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16">
+    <row r="38" spans="1:4" ht="17.399999999999999">
       <c r="A38" s="12" t="s">
         <v>556</v>
       </c>
@@ -5150,7 +5201,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16">
+    <row r="39" spans="1:4" ht="17.399999999999999">
       <c r="A39" s="12" t="s">
         <v>557</v>
       </c>
@@ -5161,7 +5212,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16">
+    <row r="40" spans="1:4" ht="17.399999999999999">
       <c r="A40" s="5" t="s">
         <v>771</v>
       </c>
@@ -5191,13 +5242,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>188</v>
       </c>
@@ -5205,7 +5256,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -5219,7 +5270,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>362</v>
       </c>
@@ -5233,7 +5284,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
         <v>363</v>
       </c>
@@ -5247,7 +5298,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
         <v>364</v>
       </c>
@@ -5258,7 +5309,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
         <v>365</v>
       </c>
@@ -5269,7 +5320,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
         <v>366</v>
       </c>
@@ -5283,7 +5334,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
         <v>367</v>
       </c>
@@ -5294,7 +5345,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A10" s="5" t="s">
         <v>368</v>
       </c>
@@ -5305,7 +5356,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A11" s="5" t="s">
         <v>369</v>
       </c>
@@ -5316,7 +5367,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
         <v>370</v>
       </c>
@@ -5327,7 +5378,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
         <v>417</v>
       </c>
@@ -5338,7 +5389,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="5" t="s">
         <v>420</v>
       </c>
@@ -5368,20 +5419,20 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.33203125" customWidth="1"/>
-    <col min="3" max="3" width="77.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.296875" customWidth="1"/>
+    <col min="3" max="3" width="77.296875" customWidth="1"/>
+    <col min="4" max="4" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
@@ -5395,7 +5446,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>333</v>
       </c>
@@ -5409,7 +5460,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
         <v>334</v>
       </c>
@@ -5423,7 +5474,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
         <v>335</v>
       </c>
@@ -5437,7 +5488,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
         <v>336</v>
       </c>
@@ -5451,7 +5502,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
         <v>371</v>
       </c>
@@ -5465,7 +5516,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
         <v>372</v>
       </c>
@@ -5479,7 +5530,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A10" s="5" t="s">
         <v>373</v>
       </c>
@@ -5493,7 +5544,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A11" s="5" t="s">
         <v>374</v>
       </c>
@@ -5507,7 +5558,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
         <v>375</v>
       </c>
@@ -5521,7 +5572,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
         <v>376</v>
       </c>
@@ -5532,7 +5583,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="5" t="s">
         <v>377</v>
       </c>
@@ -5544,7 +5595,7 @@
       </c>
       <c r="D14" s="12"/>
     </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A15" s="5" t="s">
         <v>378</v>
       </c>
@@ -5555,7 +5606,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A16" s="5" t="s">
         <v>379</v>
       </c>
@@ -5566,7 +5617,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
         <v>380</v>
       </c>
@@ -5577,7 +5628,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A18" s="5" t="s">
         <v>381</v>
       </c>
@@ -5588,7 +5639,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A19" s="5" t="s">
         <v>382</v>
       </c>
@@ -5599,7 +5650,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A20" s="5" t="s">
         <v>383</v>
       </c>
@@ -5624,7 +5675,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A22" s="5" t="s">
         <v>385</v>
       </c>
@@ -5638,7 +5689,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A23" s="5" t="s">
         <v>386</v>
       </c>
@@ -5649,7 +5700,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A24" s="5" t="s">
         <v>387</v>
       </c>
@@ -5660,7 +5711,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A25" s="5" t="s">
         <v>388</v>
       </c>
@@ -5671,7 +5722,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A26" s="5" t="s">
         <v>389</v>
       </c>
@@ -5682,7 +5733,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A27" s="5" t="s">
         <v>390</v>
       </c>
@@ -5707,7 +5758,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A29" s="5" t="s">
         <v>392</v>
       </c>
@@ -5719,7 +5770,7 @@
       </c>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A30" s="5" t="s">
         <v>393</v>
       </c>
@@ -5730,7 +5781,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A31" s="5" t="s">
         <v>394</v>
       </c>
@@ -5741,7 +5792,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A32" s="5" t="s">
         <v>395</v>
       </c>
@@ -5755,7 +5806,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A33" s="5" t="s">
         <v>396</v>
       </c>
@@ -5766,7 +5817,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="34" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A34" s="5" t="s">
         <v>397</v>
       </c>
@@ -5777,7 +5828,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A35" s="5" t="s">
         <v>398</v>
       </c>
@@ -5788,7 +5839,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="36" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A36" s="5" t="s">
         <v>399</v>
       </c>
@@ -5799,7 +5850,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A37" s="5" t="s">
         <v>506</v>
       </c>
@@ -5810,7 +5861,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="38" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A38" s="5" t="s">
         <v>507</v>
       </c>
@@ -5824,7 +5875,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A39" s="5" t="s">
         <v>508</v>
       </c>
@@ -5838,7 +5889,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="40" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A40" s="5" t="s">
         <v>509</v>
       </c>
@@ -5849,7 +5900,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A41" s="5" t="s">
         <v>510</v>
       </c>
@@ -5860,7 +5911,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="42" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A42" s="5" t="s">
         <v>511</v>
       </c>
@@ -5871,7 +5922,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A43" s="5" t="s">
         <v>447</v>
       </c>
@@ -5882,7 +5933,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="44" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A44" s="5" t="s">
         <v>448</v>
       </c>
@@ -5893,7 +5944,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="45" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A45" s="5" t="s">
         <v>449</v>
       </c>
@@ -5904,7 +5955,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="46" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A46" s="5" t="s">
         <v>450</v>
       </c>
@@ -5915,7 +5966,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="47" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A47" s="5" t="s">
         <v>458</v>
       </c>
@@ -5926,7 +5977,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="48" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A48" s="5" t="s">
         <v>463</v>
       </c>
@@ -5937,7 +5988,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="49" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A49" s="5" t="s">
         <v>471</v>
       </c>
@@ -5951,38 +6002,38 @@
         <v>505</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16">
+    <row r="50" spans="1:4" ht="17.399999999999999">
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" ht="16">
+    <row r="51" spans="1:4" ht="17.399999999999999">
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" ht="16">
+    <row r="52" spans="1:4" ht="17.399999999999999">
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" ht="16">
+    <row r="53" spans="1:4" ht="17.399999999999999">
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" ht="16">
+    <row r="54" spans="1:4" ht="17.399999999999999">
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" ht="16">
+    <row r="55" spans="1:4" ht="17.399999999999999">
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" ht="16">
+    <row r="56" spans="1:4" ht="17.399999999999999">
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" ht="16">
+    <row r="57" spans="1:4" ht="17.399999999999999">
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" ht="16">
+    <row r="58" spans="1:4" ht="17.399999999999999">
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" ht="16">
+    <row r="59" spans="1:4" ht="17.399999999999999">
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:4" ht="16">
+    <row r="60" spans="1:4" ht="17.399999999999999">
       <c r="D60" s="5"/>
     </row>
   </sheetData>
@@ -6004,19 +6055,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -6030,7 +6081,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="5" t="s">
         <v>400</v>
       </c>
@@ -6041,7 +6092,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="5" t="s">
         <v>401</v>
       </c>
@@ -6052,7 +6103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
         <v>402</v>
       </c>
@@ -6063,7 +6114,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
         <v>403</v>
       </c>
@@ -6074,7 +6125,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
         <v>404</v>
       </c>
@@ -6088,7 +6139,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
         <v>405</v>
       </c>
@@ -6099,7 +6150,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A10" s="5" t="s">
         <v>406</v>
       </c>
@@ -6110,7 +6161,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A11" s="5" t="s">
         <v>407</v>
       </c>
@@ -6121,7 +6172,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
         <v>408</v>
       </c>
@@ -6132,7 +6183,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
         <v>468</v>
       </c>
@@ -6143,7 +6194,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="5" t="s">
         <v>469</v>
       </c>
@@ -6172,14 +6223,14 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="59.1640625" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.19921875" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>421</v>
       </c>
@@ -6192,7 +6243,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -6206,7 +6257,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="12" customFormat="1" ht="17" thickTop="1">
+    <row r="4" spans="1:4" s="12" customFormat="1" ht="18" thickTop="1">
       <c r="A4" s="12" t="s">
         <v>474</v>
       </c>
@@ -6218,7 +6269,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" s="12" customFormat="1" ht="16">
+    <row r="5" spans="1:4" s="12" customFormat="1" ht="17.399999999999999">
       <c r="A5" s="12" t="s">
         <v>533</v>
       </c>
@@ -6230,7 +6281,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" s="12" customFormat="1" ht="16">
+    <row r="6" spans="1:4" s="12" customFormat="1" ht="17.399999999999999">
       <c r="A6" s="12" t="s">
         <v>534</v>
       </c>
@@ -6242,7 +6293,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="12" customFormat="1" ht="16">
+    <row r="7" spans="1:4" s="12" customFormat="1" ht="17.399999999999999">
       <c r="A7" s="12" t="s">
         <v>535</v>
       </c>
@@ -6254,7 +6305,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="16">
+    <row r="8" spans="1:4" ht="17.399999999999999">
       <c r="A8" s="12" t="s">
         <v>536</v>
       </c>
@@ -6266,7 +6317,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="16">
+    <row r="9" spans="1:4" ht="17.399999999999999">
       <c r="A9" s="12" t="s">
         <v>537</v>
       </c>
@@ -6278,7 +6329,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="16">
+    <row r="10" spans="1:4" ht="17.399999999999999">
       <c r="A10" s="12" t="s">
         <v>538</v>
       </c>
@@ -6290,7 +6341,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="16">
+    <row r="11" spans="1:4" ht="17.399999999999999">
       <c r="A11" s="12" t="s">
         <v>539</v>
       </c>
@@ -6302,7 +6353,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="16">
+    <row r="12" spans="1:4" ht="17.399999999999999">
       <c r="A12" s="12" t="s">
         <v>540</v>
       </c>
@@ -6313,7 +6364,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16">
+    <row r="13" spans="1:4" ht="17.399999999999999">
       <c r="A13" s="12" t="s">
         <v>541</v>
       </c>
@@ -6324,7 +6375,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="11" customFormat="1" ht="16">
+    <row r="14" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
       <c r="A14" s="11" t="s">
         <v>542</v>
       </c>
@@ -6338,7 +6389,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16">
+    <row r="15" spans="1:4" ht="17.399999999999999">
       <c r="A15" s="12" t="s">
         <v>616</v>
       </c>
@@ -6349,7 +6400,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16">
+    <row r="16" spans="1:4" ht="17.399999999999999">
       <c r="A16" s="12" t="s">
         <v>620</v>
       </c>
@@ -6363,7 +6414,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16">
+    <row r="17" spans="1:3" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
         <v>765</v>
       </c>
@@ -6374,7 +6425,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16">
+    <row r="18" spans="1:3" ht="17.399999999999999">
       <c r="B18" s="5"/>
     </row>
   </sheetData>
@@ -6392,18 +6443,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22">
+    <row r="1" spans="1:4" ht="22.8">
       <c r="B1" s="1" t="s">
         <v>421</v>
       </c>
@@ -6416,7 +6467,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" thickBot="1">
+    <row r="3" spans="1:4" ht="18.600000000000001" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>253</v>
       </c>
@@ -6430,7 +6481,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" thickTop="1">
+    <row r="4" spans="1:4" ht="16.2" thickTop="1">
       <c r="A4" t="s">
         <v>337</v>
       </c>
@@ -6455,7 +6506,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16">
+    <row r="6" spans="1:4" ht="17.399999999999999">
       <c r="A6" s="5" t="s">
         <v>339</v>
       </c>
@@ -6467,7 +6518,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16">
+    <row r="7" spans="1:4" ht="17.399999999999999">
       <c r="A7" s="5" t="s">
         <v>424</v>
       </c>
@@ -6479,7 +6530,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="16">
+    <row r="8" spans="1:4" ht="17.399999999999999">
       <c r="A8" s="5" t="s">
         <v>340</v>
       </c>
@@ -6491,7 +6542,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="16">
+    <row r="9" spans="1:4" ht="17.399999999999999">
       <c r="A9" s="5" t="s">
         <v>341</v>
       </c>
@@ -6531,7 +6582,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16">
+    <row r="12" spans="1:4" ht="17.399999999999999">
       <c r="A12" s="5" t="s">
         <v>344</v>
       </c>
@@ -6542,7 +6593,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16">
+    <row r="13" spans="1:4" ht="17.399999999999999">
       <c r="A13" s="5" t="s">
         <v>345</v>
       </c>

</xml_diff>

<commit_message>
added a few changes to cohort
Based on the discussions with Michael
</commit_message>
<xml_diff>
--- a/requirements/Enigma_requirements.xlsx
+++ b/requirements/Enigma_requirements.xlsx
@@ -2045,12 +2045,6 @@
     <t>CohortGroup, hasGeneticData, [string]</t>
   </si>
   <si>
-    <t>Describing the study design of a cohort group</t>
-  </si>
-  <si>
-    <t>CohortGroup, hasStudyDesign, [string]</t>
-  </si>
-  <si>
     <t>Project, hasStudyDesign, [string]</t>
   </si>
   <si>
@@ -2411,6 +2405,12 @@
   </si>
   <si>
     <t>Checked by Michael Feb 2019</t>
+  </si>
+  <si>
+    <t>Describing the study design of a cohort group/cohort</t>
+  </si>
+  <si>
+    <t>CohortGroup/Chohort/Project, hasStudyDesign, [string]</t>
   </si>
 </sst>
 </file>
@@ -3335,8 +3335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3351,13 +3351,13 @@
         <v>6</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.8">
       <c r="B2" s="2"/>
       <c r="C2" s="8" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1">
@@ -3613,7 +3613,7 @@
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="8" customFormat="1">
@@ -3897,17 +3897,17 @@
         <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="8" customFormat="1">
-      <c r="A52" s="8" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>301</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3999,14 +3999,14 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="8" customFormat="1">
-      <c r="A61" s="8" t="s">
+    <row r="61" spans="1:3" s="5" customFormat="1" ht="17.399999999999999">
+      <c r="A61" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="5" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4040,7 +4040,7 @@
         <v>93</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -4051,7 +4051,7 @@
         <v>94</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -4106,10 +4106,10 @@
         <v>319</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>663</v>
+        <v>777</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>664</v>
+        <v>778</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="8" customFormat="1">
@@ -4332,10 +4332,10 @@
         <v>653</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C90" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="17.399999999999999">
@@ -4343,10 +4343,10 @@
         <v>654</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C91" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="17.399999999999999">
@@ -4354,10 +4354,10 @@
         <v>655</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C92" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="17.399999999999999">
@@ -4365,10 +4365,10 @@
         <v>656</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C93" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="17.399999999999999">
@@ -4376,10 +4376,10 @@
         <v>657</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C94" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="17.399999999999999">
@@ -4387,10 +4387,10 @@
         <v>658</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C95" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="17.399999999999999">
@@ -4398,10 +4398,10 @@
         <v>659</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C96" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="17.399999999999999">
@@ -4409,10 +4409,10 @@
         <v>660</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="C97" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="11" customFormat="1" ht="17.399999999999999">
@@ -4420,305 +4420,305 @@
         <v>661</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>662</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="17.399999999999999">
       <c r="A99" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C99" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="17.399999999999999">
       <c r="A100" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C100" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A101" s="5" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B101" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="C101" s="5" t="s">
         <v>679</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A102" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="C102" s="5" t="s">
         <v>674</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>678</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
       <c r="A103" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="C103" s="5" t="s">
         <v>675</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>680</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="17.399999999999999">
       <c r="A104" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="B104" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="B104" s="5" t="s">
-        <v>684</v>
-      </c>
       <c r="C104" s="5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="17.399999999999999">
       <c r="A105" s="5" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="17.399999999999999">
       <c r="A106" s="5" t="s">
+        <v>688</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="C106" s="5" t="s">
         <v>690</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>691</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="17.399999999999999">
       <c r="A107" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="B107" t="s">
+        <v>708</v>
+      </c>
+      <c r="C107" s="5" t="s">
         <v>709</v>
-      </c>
-      <c r="B107" t="s">
-        <v>710</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="17.399999999999999">
       <c r="A108" s="5" t="s">
+        <v>711</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>713</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>714</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="17.399999999999999">
       <c r="A109" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>716</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>717</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="17.399999999999999">
       <c r="A110" s="5" t="s">
+        <v>717</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>721</v>
-      </c>
       <c r="C110" s="5" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="17.399999999999999">
       <c r="A111" s="5" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="17.399999999999999">
       <c r="A112" s="5" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="17.399999999999999">
       <c r="A113" s="5" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="17.399999999999999">
       <c r="A114" s="5" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="17.399999999999999">
       <c r="A115" s="5" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="17.399999999999999">
       <c r="A116" s="5" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="17.399999999999999">
       <c r="A117" s="5" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="17.399999999999999">
       <c r="A118" s="5" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="17.399999999999999">
       <c r="A119" s="5" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="17.399999999999999">
       <c r="A120" s="5" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="17.399999999999999">
       <c r="A121" s="5" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="17.399999999999999">
       <c r="A122" s="5" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="17.399999999999999">
       <c r="A124" s="5" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C124" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="D124" s="5" t="s">
         <v>774</v>
-      </c>
-      <c r="D124" s="5" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="17.399999999999999">
       <c r="A125" s="5" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B125" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="C125" s="5" t="s">
         <v>773</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -5065,7 +5065,7 @@
         <v>150</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -5214,7 +5214,7 @@
     </row>
     <row r="40" spans="1:4" ht="17.399999999999999">
       <c r="A40" s="5" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>426</v>
@@ -5803,7 +5803,7 @@
         <v>466</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="17.399999999999999">
@@ -6416,13 +6416,13 @@
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>763</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>764</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17.399999999999999">
@@ -6489,7 +6489,7 @@
         <v>586</v>
       </c>
       <c r="D4" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="11" customFormat="1">
@@ -6503,7 +6503,7 @@
         <v>588</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.399999999999999">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.399999999999999">
@@ -6538,7 +6538,7 @@
         <v>428</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D8" s="5"/>
     </row>

</xml_diff>